<commit_message>
more chapter icons and chapter data thru book 3
</commit_message>
<xml_diff>
--- a/Data/Chapters.xlsx
+++ b/Data/Chapters.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="194">
   <si>
     <t>BookTitle</t>
   </si>
@@ -38,9 +38,6 @@
     <t>ChapterIcon</t>
   </si>
   <si>
-    <t>images/chapter/</t>
-  </si>
-  <si>
     <t>IsPrologue</t>
   </si>
   <si>
@@ -213,6 +210,402 @@
   </si>
   <si>
     <t>The Great Hunt</t>
+  </si>
+  <si>
+    <t>In the Shadow</t>
+  </si>
+  <si>
+    <t>The Flame of Tar Valon</t>
+  </si>
+  <si>
+    <t>The Welcome</t>
+  </si>
+  <si>
+    <t>Friends and Enemies</t>
+  </si>
+  <si>
+    <t>Summoned</t>
+  </si>
+  <si>
+    <t>The Shadow in Shienar</t>
+  </si>
+  <si>
+    <t>Dark Prophecy</t>
+  </si>
+  <si>
+    <t>Blood Calls Blood</t>
+  </si>
+  <si>
+    <t>The Dragon Reborn</t>
+  </si>
+  <si>
+    <t>Leavetakings</t>
+  </si>
+  <si>
+    <t>The Hunt Begins</t>
+  </si>
+  <si>
+    <t>Glimmers of the Pattern</t>
+  </si>
+  <si>
+    <t>Woven in the Pattern</t>
+  </si>
+  <si>
+    <t>From Stone to Stone</t>
+  </si>
+  <si>
+    <t>Kinslayer</t>
+  </si>
+  <si>
+    <t>In the Mirror of Darkness</t>
+  </si>
+  <si>
+    <t>To the White Tower</t>
+  </si>
+  <si>
+    <t>Beneath the Dagger</t>
+  </si>
+  <si>
+    <t>Saidin</t>
+  </si>
+  <si>
+    <t>The Nine Rings</t>
+  </si>
+  <si>
+    <t>Watchers</t>
+  </si>
+  <si>
+    <t>The Testing</t>
+  </si>
+  <si>
+    <t>New Friends and Old Enemies</t>
+  </si>
+  <si>
+    <t>Cairhien</t>
+  </si>
+  <si>
+    <t>Discord</t>
+  </si>
+  <si>
+    <t>The Shadow in the Night</t>
+  </si>
+  <si>
+    <t>A New Thread in the Pattern</t>
+  </si>
+  <si>
+    <t>Seanchan</t>
+  </si>
+  <si>
+    <t>Daes Dae'mar</t>
+  </si>
+  <si>
+    <t>On the Scent</t>
+  </si>
+  <si>
+    <t>Dangerous Words</t>
+  </si>
+  <si>
+    <t>A Message from the Dark</t>
+  </si>
+  <si>
+    <t>The Wheel Weaves</t>
+  </si>
+  <si>
+    <t>Stedding Tsofu</t>
+  </si>
+  <si>
+    <t>Among the Elders</t>
+  </si>
+  <si>
+    <t>What Might Be</t>
+  </si>
+  <si>
+    <t>Practice</t>
+  </si>
+  <si>
+    <t>Flight From the White Tower</t>
+  </si>
+  <si>
+    <t>Damane</t>
+  </si>
+  <si>
+    <t>Disagreements</t>
+  </si>
+  <si>
+    <t>Falme</t>
+  </si>
+  <si>
+    <t>A Plan</t>
+  </si>
+  <si>
+    <t>Five Will Ride Forth</t>
+  </si>
+  <si>
+    <t>Blademaster</t>
+  </si>
+  <si>
+    <t>To Come Out of the Shadow</t>
+  </si>
+  <si>
+    <t>The Grave Is No Bar to My Call</t>
+  </si>
+  <si>
+    <t>First Claiming</t>
+  </si>
+  <si>
+    <t>What Was Meant to Be</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Fortress of the Light</t>
+  </si>
+  <si>
+    <t>Waiting</t>
+  </si>
+  <si>
+    <t>News from the Plain</t>
+  </si>
+  <si>
+    <t>Shadows Sleeping</t>
+  </si>
+  <si>
+    <t>Nightmares Walking</t>
+  </si>
+  <si>
+    <t>The Way Out of the Mountains</t>
+  </si>
+  <si>
+    <t>Jarra</t>
+  </si>
+  <si>
+    <t>Wolf Dreams</t>
+  </si>
+  <si>
+    <t>Secrets</t>
+  </si>
+  <si>
+    <t>Tar Valon</t>
+  </si>
+  <si>
+    <t>The Amyrlin Seat</t>
+  </si>
+  <si>
+    <t>Punishments</t>
+  </si>
+  <si>
+    <t>The Bite of the Thorns</t>
+  </si>
+  <si>
+    <t>The Gray Man</t>
+  </si>
+  <si>
+    <t>Hunters Three</t>
+  </si>
+  <si>
+    <t>The Red Sister</t>
+  </si>
+  <si>
+    <t>Healing</t>
+  </si>
+  <si>
+    <t>Awakening</t>
+  </si>
+  <si>
+    <t>Visitations</t>
+  </si>
+  <si>
+    <t>A World of Dreams</t>
+  </si>
+  <si>
+    <t>The Price of the Ring</t>
+  </si>
+  <si>
+    <t>Sealed</t>
+  </si>
+  <si>
+    <t>Scouting and Discoveries</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>Behind a Lock</t>
+  </si>
+  <si>
+    <t>Tel'aran'rhiod</t>
+  </si>
+  <si>
+    <t>A Way Out</t>
+  </si>
+  <si>
+    <t>A Trap to Spring</t>
+  </si>
+  <si>
+    <t>The First Toss</t>
+  </si>
+  <si>
+    <t>The Woman of Tanchico</t>
+  </si>
+  <si>
+    <t>The First Ship</t>
+  </si>
+  <si>
+    <t>Within the Weave</t>
+  </si>
+  <si>
+    <t>A Different Dance</t>
+  </si>
+  <si>
+    <t>The Falcon</t>
+  </si>
+  <si>
+    <t>Daughter of the Night</t>
+  </si>
+  <si>
+    <t>Fires in Cairhien</t>
+  </si>
+  <si>
+    <t>Maidens of the Spear</t>
+  </si>
+  <si>
+    <t>Threads in the Pattern</t>
+  </si>
+  <si>
+    <t>A Hero in the Night</t>
+  </si>
+  <si>
+    <t>A Hunter's Oath</t>
+  </si>
+  <si>
+    <t>Easing the Badger</t>
+  </si>
+  <si>
+    <t>Shadowbrothers</t>
+  </si>
+  <si>
+    <t>Hunted</t>
+  </si>
+  <si>
+    <t>A Message Out of the Shadow</t>
+  </si>
+  <si>
+    <t>To Race the Shadow</t>
+  </si>
+  <si>
+    <t>Following the Craft</t>
+  </si>
+  <si>
+    <t>A Storm in Tear</t>
+  </si>
+  <si>
+    <t>The Hammer</t>
+  </si>
+  <si>
+    <t>Bait for the Net</t>
+  </si>
+  <si>
+    <t>In Search of a Remedy</t>
+  </si>
+  <si>
+    <t>A Flow of the Spirit</t>
+  </si>
+  <si>
+    <t>Into the Stone</t>
+  </si>
+  <si>
+    <t>What Is Written in Prophecy</t>
+  </si>
+  <si>
+    <t>People of the Dragon</t>
+  </si>
+  <si>
+    <t>Wheel-icon.svg</t>
+  </si>
+  <si>
+    <t>Ravens-icon.svg</t>
+  </si>
+  <si>
+    <t>Fang-icon.svg</t>
+  </si>
+  <si>
+    <t>Harp-icon.svg</t>
+  </si>
+  <si>
+    <t>Deadtree-icon.svg</t>
+  </si>
+  <si>
+    <t>Hilttall-icon.svg</t>
+  </si>
+  <si>
+    <t>Staff-icon.svg</t>
+  </si>
+  <si>
+    <t>Flame-icon.svg</t>
+  </si>
+  <si>
+    <t>Cotl-icon.svg</t>
+  </si>
+  <si>
+    <t>Leaf-icon.svg</t>
+  </si>
+  <si>
+    <t>Trolloc-icon.svg</t>
+  </si>
+  <si>
+    <t>Wolf-icon.svg</t>
+  </si>
+  <si>
+    <t>Andoran-icon.svg</t>
+  </si>
+  <si>
+    <t>Blight-icon.svg</t>
+  </si>
+  <si>
+    <t>Dagger-icon.svg</t>
+  </si>
+  <si>
+    <t>Valere-icon.svg</t>
+  </si>
+  <si>
+    <t>Portal-icon.svg</t>
+  </si>
+  <si>
+    <t>Cairhien-icon.svg</t>
+  </si>
+  <si>
+    <t>Seanchan-icon.svg</t>
+  </si>
+  <si>
+    <t>Leaves-icon.svg</t>
+  </si>
+  <si>
+    <t>Tree-icon.svg</t>
+  </si>
+  <si>
+    <t>A'dam-icon.svg</t>
+  </si>
+  <si>
+    <t>Faces-icon.svg</t>
+  </si>
+  <si>
+    <t>Dice-icon.svg</t>
+  </si>
+  <si>
+    <t>Lanfear-icon.svg</t>
+  </si>
+  <si>
+    <t>Telaran-icon.svg</t>
+  </si>
+  <si>
+    <t>Waves-icon.svg</t>
+  </si>
+  <si>
+    <t>Lanfearrev-icon.svg</t>
+  </si>
+  <si>
+    <t>Dragon-icon.svg</t>
   </si>
 </sst>
 </file>
@@ -530,18 +923,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -560,21 +953,21 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>165</v>
       </c>
       <c r="E2" t="b">
         <v>1</v>
@@ -585,15 +978,18 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <f>C2+1</f>
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>165</v>
+      </c>
       <c r="E3" t="b">
         <v>0</v>
       </c>
@@ -603,15 +999,18 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C56" si="0">C3+1</f>
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>166</v>
+      </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
@@ -621,14 +1020,17 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
         <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>167</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -639,14 +1041,17 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
         <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>168</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -657,14 +1062,17 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
         <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>169</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -675,14 +1083,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
         <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>170</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -693,14 +1104,17 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
         <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>169</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -711,14 +1125,17 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
         <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>171</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -729,14 +1146,17 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
         <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>167</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -747,14 +1167,17 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>10</v>
+      <c r="D12" t="s">
+        <v>171</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -765,14 +1188,17 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
         <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>169</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -783,14 +1209,17 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
         <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>172</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -801,14 +1230,17 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
         <v>13</v>
+      </c>
+      <c r="D15" t="s">
+        <v>171</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -819,14 +1251,17 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
         <v>14</v>
+      </c>
+      <c r="D16" t="s">
+        <v>167</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -837,14 +1272,17 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
         <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>173</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -855,14 +1293,17 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
         <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>174</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -873,14 +1314,17 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
         <v>17</v>
+      </c>
+      <c r="D19" t="s">
+        <v>167</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -891,14 +1335,17 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
         <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>175</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -909,14 +1356,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
         <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>166</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -927,14 +1377,17 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
         <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>175</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -945,14 +1398,17 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
         <v>21</v>
+      </c>
+      <c r="D23" t="s">
+        <v>171</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -963,14 +1419,17 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
         <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>169</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -981,14 +1440,17 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
         <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>176</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -999,14 +1461,17 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
         <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>168</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1017,14 +1482,17 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
         <v>25</v>
+      </c>
+      <c r="D27" t="s">
+        <v>174</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1035,14 +1503,17 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
         <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>168</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1053,14 +1524,17 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
         <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>174</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1071,14 +1545,17 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
         <v>28</v>
+      </c>
+      <c r="D30" t="s">
+        <v>171</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1089,14 +1566,17 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
         <v>29</v>
+      </c>
+      <c r="D31" t="s">
+        <v>176</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1107,14 +1587,17 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
         <v>30</v>
+      </c>
+      <c r="D32" t="s">
+        <v>176</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1125,14 +1608,17 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
         <v>31</v>
+      </c>
+      <c r="D33" t="s">
+        <v>170</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1143,14 +1629,17 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
         <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>167</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1161,14 +1650,17 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
         <v>33</v>
+      </c>
+      <c r="D35" t="s">
+        <v>170</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1179,14 +1671,17 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
         <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>175</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1197,14 +1692,17 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
         <v>35</v>
+      </c>
+      <c r="D37" t="s">
+        <v>177</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1215,14 +1713,17 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
         <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>174</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1233,14 +1734,17 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
         <v>37</v>
+      </c>
+      <c r="D39" t="s">
+        <v>173</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1251,14 +1755,17 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
         <v>38</v>
+      </c>
+      <c r="D40" t="s">
+        <v>172</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1269,14 +1776,17 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
         <v>39</v>
+      </c>
+      <c r="D41" t="s">
+        <v>177</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1287,14 +1797,17 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
         <v>40</v>
+      </c>
+      <c r="D42" t="s">
+        <v>172</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1305,14 +1818,17 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
         <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>171</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1323,14 +1839,17 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
         <v>42</v>
+      </c>
+      <c r="D44" t="s">
+        <v>166</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1341,14 +1860,17 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
         <v>43</v>
+      </c>
+      <c r="D45" t="s">
+        <v>167</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -1359,14 +1881,17 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
         <v>44</v>
+      </c>
+      <c r="D46" t="s">
+        <v>174</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1377,14 +1902,17 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
         <v>45</v>
+      </c>
+      <c r="D47" t="s">
+        <v>167</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
@@ -1395,14 +1923,17 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
         <v>46</v>
+      </c>
+      <c r="D48" t="s">
+        <v>169</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1413,14 +1944,17 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
         <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>166</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1431,14 +1965,17 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
         <v>48</v>
+      </c>
+      <c r="D50" t="s">
+        <v>178</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1449,14 +1986,17 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
         <v>49</v>
+      </c>
+      <c r="D51" t="s">
+        <v>178</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -1467,14 +2007,17 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
         <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>174</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -1485,14 +2028,17 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
         <v>51</v>
+      </c>
+      <c r="D53" t="s">
+        <v>170</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -1503,14 +2049,17 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
         <v>52</v>
+      </c>
+      <c r="D54" t="s">
+        <v>174</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -1521,14 +2070,17 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
         <v>53</v>
+      </c>
+      <c r="D55" t="s">
+        <v>165</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -1539,7 +2091,2262 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56" t="s">
         <v>62</v>
+      </c>
+      <c r="D56" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" t="b">
+        <v>1</v>
+      </c>
+      <c r="F56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>61</v>
+      </c>
+      <c r="B57" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57">
+        <f>C56+1</f>
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>165</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>61</v>
+      </c>
+      <c r="B58" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58">
+        <f t="shared" ref="C58:C106" si="1">C57+1</f>
+        <v>2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+      <c r="F58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>179</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+      <c r="F59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>67</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D61" t="s">
+        <v>173</v>
+      </c>
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
+      <c r="F61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>175</v>
+      </c>
+      <c r="E62" t="b">
+        <v>0</v>
+      </c>
+      <c r="F62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>69</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>165</v>
+      </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
+      <c r="F63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D64" t="s">
+        <v>167</v>
+      </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
+      <c r="F64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>61</v>
+      </c>
+      <c r="B65" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>172</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+      <c r="F65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+      <c r="B66" t="s">
+        <v>72</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="D66" t="s">
+        <v>180</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+      <c r="F66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="D67" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>61</v>
+      </c>
+      <c r="B68" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>172</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+      <c r="F68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>61</v>
+      </c>
+      <c r="B69" t="s">
+        <v>75</v>
+      </c>
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="D69" t="s">
+        <v>181</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+      <c r="F69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>61</v>
+      </c>
+      <c r="B70" t="s">
+        <v>31</v>
+      </c>
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="D70" t="s">
+        <v>176</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+      <c r="F70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
+        <v>170</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+      <c r="F71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>61</v>
+      </c>
+      <c r="B72" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="D72" t="s">
+        <v>167</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+      <c r="F72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>61</v>
+      </c>
+      <c r="B73" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="D73" t="s">
+        <v>181</v>
+      </c>
+      <c r="E73" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="D74" t="s">
+        <v>172</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+      <c r="F74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>61</v>
+      </c>
+      <c r="B75" t="s">
+        <v>79</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="D75" t="s">
+        <v>180</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+      <c r="F75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>61</v>
+      </c>
+      <c r="B76" t="s">
+        <v>80</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="D76" t="s">
+        <v>167</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="D77" t="s">
+        <v>168</v>
+      </c>
+      <c r="E77" t="b">
+        <v>0</v>
+      </c>
+      <c r="F77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>61</v>
+      </c>
+      <c r="B78" t="s">
+        <v>82</v>
+      </c>
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="D78" t="s">
+        <v>179</v>
+      </c>
+      <c r="E78" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>61</v>
+      </c>
+      <c r="B79" t="s">
+        <v>83</v>
+      </c>
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="D79" t="s">
+        <v>172</v>
+      </c>
+      <c r="E79" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>61</v>
+      </c>
+      <c r="B80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="D80" t="s">
+        <v>172</v>
+      </c>
+      <c r="E80" t="b">
+        <v>0</v>
+      </c>
+      <c r="F80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>61</v>
+      </c>
+      <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="D81" t="s">
+        <v>182</v>
+      </c>
+      <c r="E81" t="b">
+        <v>0</v>
+      </c>
+      <c r="F81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>61</v>
+      </c>
+      <c r="B82" t="s">
+        <v>86</v>
+      </c>
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="D82" t="s">
+        <v>168</v>
+      </c>
+      <c r="E82" t="b">
+        <v>0</v>
+      </c>
+      <c r="F82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>61</v>
+      </c>
+      <c r="B83" t="s">
+        <v>87</v>
+      </c>
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="D83" t="s">
+        <v>175</v>
+      </c>
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+      <c r="F83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>61</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="D84" t="s">
+        <v>176</v>
+      </c>
+      <c r="E84" t="b">
+        <v>0</v>
+      </c>
+      <c r="F84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>61</v>
+      </c>
+      <c r="B85" t="s">
+        <v>89</v>
+      </c>
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="D85" t="s">
+        <v>183</v>
+      </c>
+      <c r="E85" t="b">
+        <v>0</v>
+      </c>
+      <c r="F85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>61</v>
+      </c>
+      <c r="B86" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D86" t="s">
+        <v>182</v>
+      </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
+      <c r="F86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>61</v>
+      </c>
+      <c r="B87" t="s">
+        <v>91</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="D87" t="s">
+        <v>182</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+      <c r="F87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>61</v>
+      </c>
+      <c r="B88" t="s">
+        <v>92</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="D88" t="s">
+        <v>168</v>
+      </c>
+      <c r="E88" t="b">
+        <v>0</v>
+      </c>
+      <c r="F88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>61</v>
+      </c>
+      <c r="B89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="D89" t="s">
+        <v>184</v>
+      </c>
+      <c r="E89" t="b">
+        <v>0</v>
+      </c>
+      <c r="F89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>61</v>
+      </c>
+      <c r="B90" t="s">
+        <v>94</v>
+      </c>
+      <c r="C90">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="D90" t="s">
+        <v>165</v>
+      </c>
+      <c r="E90" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>61</v>
+      </c>
+      <c r="B91" t="s">
+        <v>95</v>
+      </c>
+      <c r="C91">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="D91" t="s">
+        <v>185</v>
+      </c>
+      <c r="E91" t="b">
+        <v>0</v>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>61</v>
+      </c>
+      <c r="B92" t="s">
+        <v>96</v>
+      </c>
+      <c r="C92">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="D92" t="s">
+        <v>184</v>
+      </c>
+      <c r="E92" t="b">
+        <v>0</v>
+      </c>
+      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>61</v>
+      </c>
+      <c r="B93" t="s">
+        <v>97</v>
+      </c>
+      <c r="C93">
+        <f>C92+1</f>
+        <v>37</v>
+      </c>
+      <c r="D93" t="s">
+        <v>181</v>
+      </c>
+      <c r="E93" t="b">
+        <v>0</v>
+      </c>
+      <c r="F93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>61</v>
+      </c>
+      <c r="B94" t="s">
+        <v>98</v>
+      </c>
+      <c r="C94">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="D94" t="s">
+        <v>172</v>
+      </c>
+      <c r="E94" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>61</v>
+      </c>
+      <c r="B95" t="s">
+        <v>99</v>
+      </c>
+      <c r="C95">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="D95" t="s">
+        <v>184</v>
+      </c>
+      <c r="E95" t="b">
+        <v>0</v>
+      </c>
+      <c r="F95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>61</v>
+      </c>
+      <c r="B96" t="s">
+        <v>100</v>
+      </c>
+      <c r="C96">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="D96" t="s">
+        <v>186</v>
+      </c>
+      <c r="E96" t="b">
+        <v>0</v>
+      </c>
+      <c r="F96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>61</v>
+      </c>
+      <c r="B97" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="D97" t="s">
+        <v>179</v>
+      </c>
+      <c r="E97" t="b">
+        <v>0</v>
+      </c>
+      <c r="F97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>61</v>
+      </c>
+      <c r="B98" t="s">
+        <v>102</v>
+      </c>
+      <c r="C98">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="D98" t="s">
+        <v>183</v>
+      </c>
+      <c r="E98" t="b">
+        <v>0</v>
+      </c>
+      <c r="F98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>61</v>
+      </c>
+      <c r="B99" t="s">
+        <v>103</v>
+      </c>
+      <c r="C99">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="D99" t="s">
+        <v>186</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+      <c r="F99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>61</v>
+      </c>
+      <c r="B100" t="s">
+        <v>104</v>
+      </c>
+      <c r="C100">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="D100" t="s">
+        <v>172</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+      <c r="F100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>61</v>
+      </c>
+      <c r="B101" t="s">
+        <v>105</v>
+      </c>
+      <c r="C101">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="D101" t="s">
+        <v>170</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>61</v>
+      </c>
+      <c r="B102" t="s">
+        <v>106</v>
+      </c>
+      <c r="C102">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="D102" t="s">
+        <v>179</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+      <c r="F102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>61</v>
+      </c>
+      <c r="B103" t="s">
+        <v>107</v>
+      </c>
+      <c r="C103">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="D103" t="s">
+        <v>180</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104" t="s">
+        <v>108</v>
+      </c>
+      <c r="C104">
+        <f>C103+1</f>
+        <v>48</v>
+      </c>
+      <c r="D104" t="s">
+        <v>167</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+      <c r="F104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>61</v>
+      </c>
+      <c r="B105" t="s">
+        <v>109</v>
+      </c>
+      <c r="C105">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="D105" t="s">
+        <v>165</v>
+      </c>
+      <c r="E105" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>61</v>
+      </c>
+      <c r="B106" t="s">
+        <v>110</v>
+      </c>
+      <c r="C106">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="D106" t="s">
+        <v>165</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>70</v>
+      </c>
+      <c r="B107" t="s">
+        <v>111</v>
+      </c>
+      <c r="D107" t="s">
+        <v>173</v>
+      </c>
+      <c r="E107" t="b">
+        <v>1</v>
+      </c>
+      <c r="F107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>70</v>
+      </c>
+      <c r="B108" t="s">
+        <v>112</v>
+      </c>
+      <c r="C108">
+        <f>C107+1</f>
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
+        <v>166</v>
+      </c>
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+      <c r="F108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>70</v>
+      </c>
+      <c r="B109" t="s">
+        <v>80</v>
+      </c>
+      <c r="C109">
+        <f t="shared" ref="C109:C163" si="2">C108+1</f>
+        <v>2</v>
+      </c>
+      <c r="D109" t="s">
+        <v>167</v>
+      </c>
+      <c r="E109" t="b">
+        <v>0</v>
+      </c>
+      <c r="F109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>70</v>
+      </c>
+      <c r="B110" t="s">
+        <v>113</v>
+      </c>
+      <c r="C110">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="D110" t="s">
+        <v>165</v>
+      </c>
+      <c r="E110" t="b">
+        <v>0</v>
+      </c>
+      <c r="F110" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>70</v>
+      </c>
+      <c r="B111" t="s">
+        <v>114</v>
+      </c>
+      <c r="C111">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D111" t="s">
+        <v>176</v>
+      </c>
+      <c r="E111" t="b">
+        <v>0</v>
+      </c>
+      <c r="F111" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>70</v>
+      </c>
+      <c r="B112" t="s">
+        <v>115</v>
+      </c>
+      <c r="C112">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D112" t="s">
+        <v>175</v>
+      </c>
+      <c r="E112" t="b">
+        <v>0</v>
+      </c>
+      <c r="F112" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>70</v>
+      </c>
+      <c r="B113" t="s">
+        <v>72</v>
+      </c>
+      <c r="C113">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="D113" t="s">
+        <v>165</v>
+      </c>
+      <c r="E113" t="b">
+        <v>0</v>
+      </c>
+      <c r="F113" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>70</v>
+      </c>
+      <c r="B114" t="s">
+        <v>116</v>
+      </c>
+      <c r="C114">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="D114" t="s">
+        <v>172</v>
+      </c>
+      <c r="E114" t="b">
+        <v>0</v>
+      </c>
+      <c r="F114" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>70</v>
+      </c>
+      <c r="B115" t="s">
+        <v>117</v>
+      </c>
+      <c r="C115">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>176</v>
+      </c>
+      <c r="E115" t="b">
+        <v>0</v>
+      </c>
+      <c r="F115" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>70</v>
+      </c>
+      <c r="B116" t="s">
+        <v>118</v>
+      </c>
+      <c r="C116">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="D116" t="s">
+        <v>167</v>
+      </c>
+      <c r="E116" t="b">
+        <v>0</v>
+      </c>
+      <c r="F116" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>70</v>
+      </c>
+      <c r="B117" t="s">
+        <v>119</v>
+      </c>
+      <c r="C117">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="D117" t="s">
+        <v>173</v>
+      </c>
+      <c r="E117" t="b">
+        <v>0</v>
+      </c>
+      <c r="F117" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>70</v>
+      </c>
+      <c r="B118" t="s">
+        <v>120</v>
+      </c>
+      <c r="C118">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="D118" t="s">
+        <v>172</v>
+      </c>
+      <c r="E118" t="b">
+        <v>0</v>
+      </c>
+      <c r="F118" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>70</v>
+      </c>
+      <c r="B119" t="s">
+        <v>121</v>
+      </c>
+      <c r="C119">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D119" t="s">
+        <v>172</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>70</v>
+      </c>
+      <c r="B120" t="s">
+        <v>122</v>
+      </c>
+      <c r="C120">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="D120" t="s">
+        <v>172</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>70</v>
+      </c>
+      <c r="B121" t="s">
+        <v>123</v>
+      </c>
+      <c r="C121">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="D121" t="s">
+        <v>187</v>
+      </c>
+      <c r="E121" t="b">
+        <v>0</v>
+      </c>
+      <c r="F121" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>70</v>
+      </c>
+      <c r="B122" t="s">
+        <v>124</v>
+      </c>
+      <c r="C122">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D122" t="s">
+        <v>187</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>70</v>
+      </c>
+      <c r="B123" t="s">
+        <v>125</v>
+      </c>
+      <c r="C123">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="D123" t="s">
+        <v>177</v>
+      </c>
+      <c r="E123" t="b">
+        <v>0</v>
+      </c>
+      <c r="F123" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>70</v>
+      </c>
+      <c r="B124" t="s">
+        <v>126</v>
+      </c>
+      <c r="C124">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="D124" t="s">
+        <v>172</v>
+      </c>
+      <c r="E124" t="b">
+        <v>0</v>
+      </c>
+      <c r="F124" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>70</v>
+      </c>
+      <c r="B125" t="s">
+        <v>127</v>
+      </c>
+      <c r="C125">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D125" t="s">
+        <v>170</v>
+      </c>
+      <c r="E125" t="b">
+        <v>0</v>
+      </c>
+      <c r="F125" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>70</v>
+      </c>
+      <c r="B126" t="s">
+        <v>128</v>
+      </c>
+      <c r="C126">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D126" t="s">
+        <v>188</v>
+      </c>
+      <c r="E126" t="b">
+        <v>0</v>
+      </c>
+      <c r="F126" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>70</v>
+      </c>
+      <c r="B127" t="s">
+        <v>129</v>
+      </c>
+      <c r="C127">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="D127" t="s">
+        <v>189</v>
+      </c>
+      <c r="E127" t="b">
+        <v>0</v>
+      </c>
+      <c r="F127" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>70</v>
+      </c>
+      <c r="B128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C128">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D128" t="s">
+        <v>190</v>
+      </c>
+      <c r="E128" t="b">
+        <v>0</v>
+      </c>
+      <c r="F128" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>70</v>
+      </c>
+      <c r="B129" t="s">
+        <v>131</v>
+      </c>
+      <c r="C129">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="D129" t="s">
+        <v>172</v>
+      </c>
+      <c r="E129" t="b">
+        <v>0</v>
+      </c>
+      <c r="F129" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>70</v>
+      </c>
+      <c r="B130" t="s">
+        <v>132</v>
+      </c>
+      <c r="C130">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D130" t="s">
+        <v>165</v>
+      </c>
+      <c r="E130" t="b">
+        <v>0</v>
+      </c>
+      <c r="F130" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>70</v>
+      </c>
+      <c r="B131" t="s">
+        <v>133</v>
+      </c>
+      <c r="C131">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D131" t="s">
+        <v>188</v>
+      </c>
+      <c r="E131" t="b">
+        <v>0</v>
+      </c>
+      <c r="F131" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>70</v>
+      </c>
+      <c r="B132" t="s">
+        <v>134</v>
+      </c>
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="D132" t="s">
+        <v>189</v>
+      </c>
+      <c r="E132" t="b">
+        <v>0</v>
+      </c>
+      <c r="F132" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>70</v>
+      </c>
+      <c r="B133" t="s">
+        <v>135</v>
+      </c>
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="D133" t="s">
+        <v>187</v>
+      </c>
+      <c r="E133" t="b">
+        <v>0</v>
+      </c>
+      <c r="F133" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>70</v>
+      </c>
+      <c r="B134" t="s">
+        <v>136</v>
+      </c>
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D134" t="s">
+        <v>190</v>
+      </c>
+      <c r="E134" t="b">
+        <v>0</v>
+      </c>
+      <c r="F134" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>70</v>
+      </c>
+      <c r="B135" t="s">
+        <v>137</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D135" t="s">
+        <v>188</v>
+      </c>
+      <c r="E135" t="b">
+        <v>0</v>
+      </c>
+      <c r="F135" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>70</v>
+      </c>
+      <c r="B136" t="s">
+        <v>138</v>
+      </c>
+      <c r="C136">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D136" t="s">
+        <v>172</v>
+      </c>
+      <c r="E136" t="b">
+        <v>0</v>
+      </c>
+      <c r="F136" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>70</v>
+      </c>
+      <c r="B137" t="s">
+        <v>139</v>
+      </c>
+      <c r="C137">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="D137" t="s">
+        <v>188</v>
+      </c>
+      <c r="E137" t="b">
+        <v>0</v>
+      </c>
+      <c r="F137" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>70</v>
+      </c>
+      <c r="B138" t="s">
+        <v>140</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="D138" t="s">
+        <v>168</v>
+      </c>
+      <c r="E138" t="b">
+        <v>0</v>
+      </c>
+      <c r="F138" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>70</v>
+      </c>
+      <c r="B139" t="s">
+        <v>141</v>
+      </c>
+      <c r="C139">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="D139" t="s">
+        <v>191</v>
+      </c>
+      <c r="E139" t="b">
+        <v>0</v>
+      </c>
+      <c r="F139" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>70</v>
+      </c>
+      <c r="B140" t="s">
+        <v>142</v>
+      </c>
+      <c r="C140">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="D140" t="s">
+        <v>165</v>
+      </c>
+      <c r="E140" t="b">
+        <v>0</v>
+      </c>
+      <c r="F140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>70</v>
+      </c>
+      <c r="B141" t="s">
+        <v>143</v>
+      </c>
+      <c r="C141">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="D141" t="s">
+        <v>165</v>
+      </c>
+      <c r="E141" t="b">
+        <v>0</v>
+      </c>
+      <c r="F141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>70</v>
+      </c>
+      <c r="B142" t="s">
+        <v>144</v>
+      </c>
+      <c r="C142">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="D142" t="s">
+        <v>191</v>
+      </c>
+      <c r="E142" t="b">
+        <v>0</v>
+      </c>
+      <c r="F142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>70</v>
+      </c>
+      <c r="B143" t="s">
+        <v>145</v>
+      </c>
+      <c r="C143">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="D143" t="s">
+        <v>192</v>
+      </c>
+      <c r="E143" t="b">
+        <v>0</v>
+      </c>
+      <c r="F143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>70</v>
+      </c>
+      <c r="B144" t="s">
+        <v>146</v>
+      </c>
+      <c r="C144">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="D144" t="s">
+        <v>182</v>
+      </c>
+      <c r="E144" t="b">
+        <v>0</v>
+      </c>
+      <c r="F144" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>70</v>
+      </c>
+      <c r="B145" t="s">
+        <v>147</v>
+      </c>
+      <c r="C145">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="D145" t="s">
+        <v>165</v>
+      </c>
+      <c r="E145" t="b">
+        <v>0</v>
+      </c>
+      <c r="F145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>70</v>
+      </c>
+      <c r="B146" t="s">
+        <v>148</v>
+      </c>
+      <c r="C146">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="D146" t="s">
+        <v>165</v>
+      </c>
+      <c r="E146" t="b">
+        <v>0</v>
+      </c>
+      <c r="F146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>70</v>
+      </c>
+      <c r="B147" t="s">
+        <v>149</v>
+      </c>
+      <c r="C147">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="D147" t="s">
+        <v>177</v>
+      </c>
+      <c r="E147" t="b">
+        <v>0</v>
+      </c>
+      <c r="F147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>70</v>
+      </c>
+      <c r="B148" t="s">
+        <v>150</v>
+      </c>
+      <c r="C148">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="D148" t="s">
+        <v>176</v>
+      </c>
+      <c r="E148" t="b">
+        <v>0</v>
+      </c>
+      <c r="F148" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>70</v>
+      </c>
+      <c r="B149" t="s">
+        <v>151</v>
+      </c>
+      <c r="C149">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="D149" t="s">
+        <v>167</v>
+      </c>
+      <c r="E149" t="b">
+        <v>0</v>
+      </c>
+      <c r="F149" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>70</v>
+      </c>
+      <c r="B150" t="s">
+        <v>152</v>
+      </c>
+      <c r="C150">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="D150" t="s">
+        <v>176</v>
+      </c>
+      <c r="E150" t="b">
+        <v>0</v>
+      </c>
+      <c r="F150" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>70</v>
+      </c>
+      <c r="B151" t="s">
+        <v>153</v>
+      </c>
+      <c r="C151">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="D151" t="s">
+        <v>172</v>
+      </c>
+      <c r="E151" t="b">
+        <v>0</v>
+      </c>
+      <c r="F151" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>70</v>
+      </c>
+      <c r="B152" t="s">
+        <v>43</v>
+      </c>
+      <c r="C152">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="D152" t="s">
+        <v>177</v>
+      </c>
+      <c r="E152" t="b">
+        <v>0</v>
+      </c>
+      <c r="F152" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>70</v>
+      </c>
+      <c r="B153" t="s">
+        <v>154</v>
+      </c>
+      <c r="C153">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="D153" t="s">
+        <v>177</v>
+      </c>
+      <c r="E153" t="b">
+        <v>0</v>
+      </c>
+      <c r="F153" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>70</v>
+      </c>
+      <c r="B154" t="s">
+        <v>155</v>
+      </c>
+      <c r="C154">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="D154" t="s">
+        <v>188</v>
+      </c>
+      <c r="E154" t="b">
+        <v>0</v>
+      </c>
+      <c r="F154" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>70</v>
+      </c>
+      <c r="B155" t="s">
+        <v>156</v>
+      </c>
+      <c r="C155">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="D155" t="s">
+        <v>184</v>
+      </c>
+      <c r="E155" t="b">
+        <v>0</v>
+      </c>
+      <c r="F155" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>70</v>
+      </c>
+      <c r="B156" t="s">
+        <v>157</v>
+      </c>
+      <c r="C156">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="D156" t="s">
+        <v>188</v>
+      </c>
+      <c r="E156" t="b">
+        <v>0</v>
+      </c>
+      <c r="F156" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>70</v>
+      </c>
+      <c r="B157" t="s">
+        <v>158</v>
+      </c>
+      <c r="C157">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="D157" t="s">
+        <v>165</v>
+      </c>
+      <c r="E157" t="b">
+        <v>0</v>
+      </c>
+      <c r="F157" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>70</v>
+      </c>
+      <c r="B158" t="s">
+        <v>159</v>
+      </c>
+      <c r="C158">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="D158" t="s">
+        <v>187</v>
+      </c>
+      <c r="E158" t="b">
+        <v>0</v>
+      </c>
+      <c r="F158" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>70</v>
+      </c>
+      <c r="B159" t="s">
+        <v>160</v>
+      </c>
+      <c r="C159">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="D159" t="s">
+        <v>168</v>
+      </c>
+      <c r="E159" t="b">
+        <v>0</v>
+      </c>
+      <c r="F159" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>70</v>
+      </c>
+      <c r="B160" t="s">
+        <v>161</v>
+      </c>
+      <c r="C160">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="D160" t="s">
+        <v>176</v>
+      </c>
+      <c r="E160" t="b">
+        <v>0</v>
+      </c>
+      <c r="F160" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>70</v>
+      </c>
+      <c r="B161" t="s">
+        <v>162</v>
+      </c>
+      <c r="C161">
+        <f>C160+1</f>
+        <v>54</v>
+      </c>
+      <c r="D161" t="s">
+        <v>188</v>
+      </c>
+      <c r="E161" t="b">
+        <v>0</v>
+      </c>
+      <c r="F161" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>70</v>
+      </c>
+      <c r="B162" t="s">
+        <v>163</v>
+      </c>
+      <c r="C162">
+        <f t="shared" si="2"/>
+        <v>55</v>
+      </c>
+      <c r="D162" t="s">
+        <v>193</v>
+      </c>
+      <c r="E162" t="b">
+        <v>0</v>
+      </c>
+      <c r="F162" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>70</v>
+      </c>
+      <c r="B163" t="s">
+        <v>164</v>
+      </c>
+      <c r="C163">
+        <f t="shared" si="2"/>
+        <v>56</v>
+      </c>
+      <c r="D163" t="s">
+        <v>165</v>
+      </c>
+      <c r="E163" t="b">
+        <v>0</v>
+      </c>
+      <c r="F163" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ChapterIcon tab in data collection
</commit_message>
<xml_diff>
--- a/Data/Chapters.xlsx
+++ b/Data/Chapters.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Chapter" sheetId="1" r:id="rId1"/>
+    <sheet name="ChapterIcon" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="195">
   <si>
     <t>BookTitle</t>
   </si>
@@ -606,6 +607,9 @@
   </si>
   <si>
     <t>Dragon-icon.svg</t>
+  </si>
+  <si>
+    <t>IconFilename</t>
   </si>
 </sst>
 </file>
@@ -925,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="A164" sqref="A164"/>
+    <sheetView topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,16 +965,20 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>100</v>
+      </c>
+      <c r="C2" t="e">
+        <f>C1+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D2" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -978,17 +986,17 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
+        <v>103</v>
+      </c>
+      <c r="C3" t="e">
         <f>C2+1</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="D3" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1002,14 +1010,14 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:C56" si="0">C3+1</f>
-        <v>2</v>
+        <v>43</v>
+      </c>
+      <c r="C4" t="e">
+        <f>C3+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D4" t="s">
-        <v>166</v>
+        <v>177</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -1023,14 +1031,14 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="C5" t="e">
+        <f>C4+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D5" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1041,17 +1049,17 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <v>125</v>
+      </c>
+      <c r="C6" t="e">
+        <f>C5+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1062,17 +1070,17 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>149</v>
+      </c>
+      <c r="C7" t="e">
+        <f>C6+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D7" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1083,17 +1091,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <v>43</v>
+      </c>
+      <c r="C8" t="e">
+        <f>C7+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1104,17 +1112,17 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <v>154</v>
+      </c>
+      <c r="C9" t="e">
+        <f>C8+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D9" t="s">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1128,14 +1136,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <v>56</v>
+      </c>
+      <c r="C10" t="e">
+        <f>C9+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D10" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1149,14 +1157,14 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <v>57</v>
+      </c>
+      <c r="C11" t="e">
+        <f>C10+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1167,17 +1175,17 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <v>85</v>
+      </c>
+      <c r="C12" t="e">
+        <f>C11+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1188,17 +1196,17 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <f t="shared" si="0"/>
-        <v>11</v>
+        <v>90</v>
+      </c>
+      <c r="C13" t="e">
+        <f>C12+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D13" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1209,17 +1217,17 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <f t="shared" si="0"/>
-        <v>12</v>
+        <v>91</v>
+      </c>
+      <c r="C14" t="e">
+        <f>C13+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D14" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1230,17 +1238,17 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <v>146</v>
+      </c>
+      <c r="C15" t="e">
+        <f>C14+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>182</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1254,14 +1262,14 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="C16" t="e">
+        <f>C15+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D16" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1275,11 +1283,11 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17">
-        <f t="shared" si="0"/>
-        <v>15</v>
+        <v>45</v>
+      </c>
+      <c r="C17" t="e">
+        <f>C16+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D17" t="s">
         <v>173</v>
@@ -1293,17 +1301,17 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>67</v>
+      </c>
+      <c r="C18" t="e">
+        <f>C17+1</f>
+        <v>#VALUE!</v>
       </c>
       <c r="D18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1314,20 +1322,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="0"/>
-        <v>17</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
-        <v>167</v>
+        <v>173</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1335,17 +1339,17 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <f>C19+1</f>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1356,17 +1360,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
-        <v>19</v>
+        <f>C20+1</f>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1377,17 +1381,17 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>82</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f>C21+1</f>
+        <v>3</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1398,17 +1402,17 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f>C22+1</f>
+        <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1419,17 +1423,17 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
-        <v>22</v>
+        <f>C23+1</f>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1443,14 +1447,14 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>C24+1</f>
+        <v>6</v>
       </c>
       <c r="D25" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1464,14 +1468,14 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
-        <v>24</v>
+        <f>C25+1</f>
+        <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1485,14 +1489,14 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
-        <v>25</v>
+        <f>C26+1</f>
+        <v>8</v>
       </c>
       <c r="D27" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1506,14 +1510,14 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
-        <v>26</v>
+        <f>C27+1</f>
+        <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1527,14 +1531,14 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
-        <v>27</v>
+        <f>C28+1</f>
+        <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1545,17 +1549,17 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
-        <v>28</v>
+        <f>C29+1</f>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1566,17 +1570,17 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
-        <v>29</v>
+        <f>C30+1</f>
+        <v>12</v>
       </c>
       <c r="D31" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1587,17 +1591,17 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>137</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
-        <v>30</v>
+        <f>C31+1</f>
+        <v>13</v>
       </c>
       <c r="D32" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1608,17 +1612,17 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="C33">
-        <f t="shared" si="0"/>
-        <v>31</v>
+        <f>C32+1</f>
+        <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1629,17 +1633,17 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
+        <v>155</v>
       </c>
       <c r="C34">
-        <f t="shared" si="0"/>
-        <v>32</v>
+        <f>C33+1</f>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1650,17 +1654,17 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="C35">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f>C34+1</f>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1671,17 +1675,17 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>162</v>
       </c>
       <c r="C36">
-        <f t="shared" si="0"/>
-        <v>34</v>
+        <f>C35+1</f>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1692,17 +1696,17 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>163</v>
       </c>
       <c r="C37">
-        <f t="shared" si="0"/>
-        <v>35</v>
+        <f>C36+1</f>
+        <v>18</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1713,17 +1717,17 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="C38">
-        <f t="shared" si="0"/>
-        <v>36</v>
+        <f>C37+1</f>
+        <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1734,17 +1738,17 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="C39">
-        <f t="shared" si="0"/>
-        <v>37</v>
+        <f>C38+1</f>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1755,17 +1759,17 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>135</v>
       </c>
       <c r="C40">
-        <f t="shared" si="0"/>
-        <v>38</v>
+        <f>C39+1</f>
+        <v>21</v>
       </c>
       <c r="D40" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1776,17 +1780,17 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>159</v>
       </c>
       <c r="C41">
-        <f t="shared" si="0"/>
-        <v>39</v>
+        <f>C40+1</f>
+        <v>22</v>
       </c>
       <c r="D41" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1800,14 +1804,14 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="C42">
-        <f t="shared" si="0"/>
-        <v>40</v>
+        <f>C41+1</f>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1821,14 +1825,14 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C43">
-        <f t="shared" si="0"/>
-        <v>41</v>
+        <f>C42+1</f>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1842,14 +1846,14 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="C44">
-        <f t="shared" si="0"/>
-        <v>42</v>
+        <f>C43+1</f>
+        <v>25</v>
       </c>
       <c r="D44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1863,11 +1867,11 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C45">
-        <f t="shared" si="0"/>
-        <v>43</v>
+        <f>C44+1</f>
+        <v>26</v>
       </c>
       <c r="D45" t="s">
         <v>167</v>
@@ -1884,14 +1888,14 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C46">
-        <f t="shared" si="0"/>
-        <v>44</v>
+        <f>C45+1</f>
+        <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1905,11 +1909,11 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C47">
-        <f t="shared" si="0"/>
-        <v>45</v>
+        <f>C46+1</f>
+        <v>28</v>
       </c>
       <c r="D47" t="s">
         <v>167</v>
@@ -1926,14 +1930,14 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48">
-        <f t="shared" si="0"/>
-        <v>46</v>
+        <f>C47+1</f>
+        <v>29</v>
       </c>
       <c r="D48" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1944,17 +1948,17 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="C49">
-        <f t="shared" si="0"/>
-        <v>47</v>
+        <f>C48+1</f>
+        <v>30</v>
       </c>
       <c r="D49" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1965,17 +1969,17 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B50" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="C50">
-        <f t="shared" si="0"/>
-        <v>48</v>
+        <f>C49+1</f>
+        <v>31</v>
       </c>
       <c r="D50" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1986,17 +1990,17 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="C51">
-        <f t="shared" si="0"/>
-        <v>49</v>
+        <f>C50+1</f>
+        <v>32</v>
       </c>
       <c r="D51" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2007,17 +2011,17 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="C52">
-        <f t="shared" si="0"/>
-        <v>50</v>
+        <f>C51+1</f>
+        <v>33</v>
       </c>
       <c r="D52" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -2028,17 +2032,17 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B53" t="s">
-        <v>59</v>
+        <v>80</v>
       </c>
       <c r="C53">
-        <f t="shared" si="0"/>
-        <v>51</v>
+        <f>C52+1</f>
+        <v>34</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -2049,17 +2053,17 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>60</v>
+        <v>118</v>
       </c>
       <c r="C54">
-        <f t="shared" si="0"/>
-        <v>52</v>
+        <f>C53+1</f>
+        <v>35</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -2070,17 +2074,17 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>8</v>
+        <v>151</v>
       </c>
       <c r="C55">
-        <f t="shared" si="0"/>
-        <v>53</v>
+        <f>C54+1</f>
+        <v>36</v>
       </c>
       <c r="D55" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -2091,16 +2095,20 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>62</v>
+        <v>20</v>
+      </c>
+      <c r="C56">
+        <f>C55+1</f>
+        <v>37</v>
       </c>
       <c r="D56" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E56" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -2108,17 +2116,17 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C57">
         <f>C56+1</f>
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
@@ -2129,14 +2137,14 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C58">
-        <f t="shared" ref="C58:C106" si="1">C57+1</f>
-        <v>2</v>
+        <f>C57+1</f>
+        <v>39</v>
       </c>
       <c r="D58" t="s">
         <v>172</v>
@@ -2153,14 +2161,14 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59">
-        <f t="shared" si="1"/>
-        <v>3</v>
+        <f>C58+1</f>
+        <v>40</v>
       </c>
       <c r="D59" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -2174,14 +2182,14 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C60">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f>C59+1</f>
+        <v>41</v>
       </c>
       <c r="D60" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -2195,14 +2203,14 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="C61">
-        <f t="shared" si="1"/>
-        <v>5</v>
+        <f>C60+1</f>
+        <v>42</v>
       </c>
       <c r="D61" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -2216,14 +2224,14 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="C62">
-        <f t="shared" si="1"/>
-        <v>6</v>
+        <f>C61+1</f>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -2237,14 +2245,14 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C63">
-        <f t="shared" si="1"/>
-        <v>7</v>
+        <f>C62+1</f>
+        <v>44</v>
       </c>
       <c r="D63" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -2258,14 +2266,14 @@
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C64">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f>C63+1</f>
+        <v>45</v>
       </c>
       <c r="D64" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -2279,11 +2287,11 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="C65">
-        <f t="shared" si="1"/>
-        <v>9</v>
+        <f>C64+1</f>
+        <v>46</v>
       </c>
       <c r="D65" t="s">
         <v>172</v>
@@ -2300,14 +2308,14 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
       <c r="C66">
-        <f t="shared" si="1"/>
-        <v>10</v>
+        <f>C65+1</f>
+        <v>47</v>
       </c>
       <c r="D66" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -2318,17 +2326,17 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>73</v>
+        <v>116</v>
       </c>
       <c r="C67">
-        <f t="shared" si="1"/>
-        <v>11</v>
+        <f>C66+1</f>
+        <v>48</v>
       </c>
       <c r="D67" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -2339,14 +2347,14 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
       <c r="C68">
-        <f t="shared" si="1"/>
-        <v>12</v>
+        <f>C67+1</f>
+        <v>49</v>
       </c>
       <c r="D68" t="s">
         <v>172</v>
@@ -2360,17 +2368,17 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>75</v>
+        <v>121</v>
       </c>
       <c r="C69">
-        <f t="shared" si="1"/>
-        <v>13</v>
+        <f>C68+1</f>
+        <v>50</v>
       </c>
       <c r="D69" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -2381,17 +2389,17 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>31</v>
+        <v>122</v>
       </c>
       <c r="C70">
-        <f t="shared" si="1"/>
-        <v>14</v>
+        <f>C69+1</f>
+        <v>51</v>
       </c>
       <c r="D70" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -2402,17 +2410,17 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="C71">
-        <f t="shared" si="1"/>
-        <v>15</v>
+        <f>C70+1</f>
+        <v>52</v>
       </c>
       <c r="D71" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -2423,17 +2431,17 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="C72">
-        <f t="shared" si="1"/>
-        <v>16</v>
+        <f>C71+1</f>
+        <v>53</v>
       </c>
       <c r="D72" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -2444,17 +2452,17 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>138</v>
       </c>
       <c r="C73">
-        <f t="shared" si="1"/>
-        <v>17</v>
+        <f>C72+1</f>
+        <v>54</v>
       </c>
       <c r="D73" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -2465,14 +2473,14 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B74" t="s">
-        <v>78</v>
+        <v>153</v>
       </c>
       <c r="C74">
-        <f t="shared" si="1"/>
-        <v>18</v>
+        <f>C73+1</f>
+        <v>55</v>
       </c>
       <c r="D74" t="s">
         <v>172</v>
@@ -2486,17 +2494,17 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>79</v>
+        <v>12</v>
       </c>
       <c r="C75">
-        <f t="shared" si="1"/>
-        <v>19</v>
+        <f>C74+1</f>
+        <v>56</v>
       </c>
       <c r="D75" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
@@ -2507,17 +2515,17 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="C76">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f>C75+1</f>
+        <v>57</v>
       </c>
       <c r="D76" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
@@ -2528,14 +2536,14 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="C77">
-        <f t="shared" si="1"/>
-        <v>21</v>
+        <f>C76+1</f>
+        <v>58</v>
       </c>
       <c r="D77" t="s">
         <v>168</v>
@@ -2552,14 +2560,14 @@
         <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C78">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f>C77+1</f>
+        <v>59</v>
       </c>
       <c r="D78" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
@@ -2573,14 +2581,14 @@
         <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C79">
-        <f t="shared" si="1"/>
-        <v>23</v>
+        <f>C78+1</f>
+        <v>60</v>
       </c>
       <c r="D79" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
@@ -2594,14 +2602,14 @@
         <v>61</v>
       </c>
       <c r="B80" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="C80">
-        <f t="shared" si="1"/>
-        <v>24</v>
+        <f>C79+1</f>
+        <v>61</v>
       </c>
       <c r="D80" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
@@ -2612,17 +2620,17 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B81" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="C81">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f>C80+1</f>
+        <v>62</v>
       </c>
       <c r="D81" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="E81" t="b">
         <v>0</v>
@@ -2633,14 +2641,14 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B82" t="s">
-        <v>86</v>
+        <v>160</v>
       </c>
       <c r="C82">
-        <f t="shared" si="1"/>
-        <v>26</v>
+        <f>C81+1</f>
+        <v>63</v>
       </c>
       <c r="D82" t="s">
         <v>168</v>
@@ -2654,17 +2662,17 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="C83">
-        <f t="shared" si="1"/>
-        <v>27</v>
+        <f>C82+1</f>
+        <v>64</v>
       </c>
       <c r="D83" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -2675,17 +2683,17 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="C84">
-        <f t="shared" si="1"/>
-        <v>28</v>
+        <f>C83+1</f>
+        <v>65</v>
       </c>
       <c r="D84" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E84" t="b">
         <v>0</v>
@@ -2696,17 +2704,17 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>89</v>
+        <v>41</v>
       </c>
       <c r="C85">
-        <f t="shared" si="1"/>
-        <v>29</v>
+        <f>C84+1</f>
+        <v>66</v>
       </c>
       <c r="D85" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
@@ -2717,17 +2725,17 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>90</v>
+        <v>59</v>
       </c>
       <c r="C86">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <f>C85+1</f>
+        <v>67</v>
       </c>
       <c r="D86" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
@@ -2741,14 +2749,14 @@
         <v>61</v>
       </c>
       <c r="B87" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="C87">
-        <f t="shared" si="1"/>
-        <v>31</v>
+        <f>C86+1</f>
+        <v>68</v>
       </c>
       <c r="D87" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="E87" t="b">
         <v>0</v>
@@ -2762,14 +2770,14 @@
         <v>61</v>
       </c>
       <c r="B88" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="C88">
-        <f t="shared" si="1"/>
-        <v>32</v>
+        <f>C87+1</f>
+        <v>69</v>
       </c>
       <c r="D88" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
@@ -2780,17 +2788,17 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B89" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="C89">
-        <f t="shared" si="1"/>
-        <v>33</v>
+        <f>C88+1</f>
+        <v>70</v>
       </c>
       <c r="D89" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="E89" t="b">
         <v>0</v>
@@ -2801,17 +2809,17 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B90" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="C90">
-        <f t="shared" si="1"/>
-        <v>34</v>
+        <f>C89+1</f>
+        <v>71</v>
       </c>
       <c r="D90" t="s">
-        <v>165</v>
+        <v>189</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
@@ -2822,17 +2830,17 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B91" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="C91">
-        <f t="shared" si="1"/>
-        <v>35</v>
+        <f>C90+1</f>
+        <v>72</v>
       </c>
       <c r="D91" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
@@ -2843,17 +2851,17 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B92" t="s">
-        <v>96</v>
+        <v>145</v>
       </c>
       <c r="C92">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f>C91+1</f>
+        <v>73</v>
       </c>
       <c r="D92" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="E92" t="b">
         <v>0</v>
@@ -2864,17 +2872,17 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="C93">
         <f>C92+1</f>
-        <v>37</v>
+        <v>74</v>
       </c>
       <c r="D93" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E93" t="b">
         <v>0</v>
@@ -2885,17 +2893,17 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="C94">
-        <f t="shared" si="1"/>
-        <v>38</v>
+        <f>C93+1</f>
+        <v>75</v>
       </c>
       <c r="D94" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
@@ -2906,17 +2914,17 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>99</v>
+        <v>35</v>
       </c>
       <c r="C95">
-        <f t="shared" si="1"/>
-        <v>39</v>
+        <f>C94+1</f>
+        <v>76</v>
       </c>
       <c r="D95" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -2927,17 +2935,17 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="C96">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f>C95+1</f>
+        <v>77</v>
       </c>
       <c r="D96" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E96" t="b">
         <v>0</v>
@@ -2948,17 +2956,17 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>101</v>
+        <v>52</v>
       </c>
       <c r="C97">
-        <f t="shared" si="1"/>
-        <v>41</v>
+        <f>C96+1</f>
+        <v>78</v>
       </c>
       <c r="D97" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
@@ -2969,17 +2977,17 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="C98">
-        <f t="shared" si="1"/>
-        <v>42</v>
+        <f>C97+1</f>
+        <v>79</v>
       </c>
       <c r="D98" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
@@ -2990,17 +2998,17 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C99">
-        <f t="shared" si="1"/>
-        <v>43</v>
+        <f>C98+1</f>
+        <v>80</v>
       </c>
       <c r="D99" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -3014,14 +3022,14 @@
         <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="C100">
-        <f t="shared" si="1"/>
-        <v>44</v>
+        <f>C99+1</f>
+        <v>81</v>
       </c>
       <c r="D100" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
@@ -3035,14 +3043,14 @@
         <v>61</v>
       </c>
       <c r="B101" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C101">
-        <f t="shared" si="1"/>
-        <v>45</v>
+        <f>C100+1</f>
+        <v>82</v>
       </c>
       <c r="D101" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
@@ -3056,14 +3064,14 @@
         <v>61</v>
       </c>
       <c r="B102" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="C102">
-        <f t="shared" si="1"/>
-        <v>46</v>
+        <f>C101+1</f>
+        <v>83</v>
       </c>
       <c r="D102" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -3074,17 +3082,17 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B103" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="C103">
-        <f t="shared" si="1"/>
-        <v>47</v>
+        <f>C102+1</f>
+        <v>84</v>
       </c>
       <c r="D103" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E103" t="b">
         <v>0</v>
@@ -3098,14 +3106,14 @@
         <v>61</v>
       </c>
       <c r="B104" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C104">
         <f>C103+1</f>
-        <v>48</v>
+        <v>85</v>
       </c>
       <c r="D104" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -3119,14 +3127,14 @@
         <v>61</v>
       </c>
       <c r="B105" t="s">
-        <v>109</v>
+        <v>21</v>
       </c>
       <c r="C105">
-        <f t="shared" si="1"/>
-        <v>49</v>
+        <f>C104+1</f>
+        <v>86</v>
       </c>
       <c r="D105" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3140,14 +3148,14 @@
         <v>61</v>
       </c>
       <c r="B106" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C106">
-        <f t="shared" si="1"/>
-        <v>50</v>
+        <f>C105+1</f>
+        <v>87</v>
       </c>
       <c r="D106" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="E106" t="b">
         <v>0</v>
@@ -3158,16 +3166,20 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>111</v>
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <f>C106+1</f>
+        <v>88</v>
       </c>
       <c r="D107" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="E107" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
@@ -3175,14 +3187,14 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>112</v>
+        <v>27</v>
       </c>
       <c r="C108">
         <f>C107+1</f>
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="D108" t="s">
         <v>166</v>
@@ -3196,17 +3208,17 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B109" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="C109">
-        <f t="shared" ref="C109:C163" si="2">C108+1</f>
-        <v>2</v>
+        <f>C108+1</f>
+        <v>90</v>
       </c>
       <c r="D109" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -3217,17 +3229,17 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="C110">
-        <f t="shared" si="2"/>
-        <v>3</v>
+        <f>C109+1</f>
+        <v>91</v>
       </c>
       <c r="D110" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E110" t="b">
         <v>0</v>
@@ -3241,14 +3253,14 @@
         <v>70</v>
       </c>
       <c r="B111" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C111">
-        <f t="shared" si="2"/>
-        <v>4</v>
+        <f>C110+1</f>
+        <v>92</v>
       </c>
       <c r="D111" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
@@ -3259,17 +3271,17 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B112" t="s">
-        <v>115</v>
+        <v>89</v>
       </c>
       <c r="C112">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f>C111+1</f>
+        <v>93</v>
       </c>
       <c r="D112" t="s">
-        <v>175</v>
+        <v>183</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
@@ -3280,17 +3292,17 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B113" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="C113">
-        <f t="shared" si="2"/>
-        <v>6</v>
+        <f>C112+1</f>
+        <v>94</v>
       </c>
       <c r="D113" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -3301,17 +3313,17 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B114" t="s">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="C114">
-        <f t="shared" si="2"/>
-        <v>7</v>
+        <f>C113+1</f>
+        <v>95</v>
       </c>
       <c r="D114" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E114" t="b">
         <v>0</v>
@@ -3322,17 +3334,17 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>117</v>
+        <v>18</v>
       </c>
       <c r="C115">
-        <f t="shared" si="2"/>
-        <v>8</v>
+        <f>C114+1</f>
+        <v>96</v>
       </c>
       <c r="D115" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E115" t="b">
         <v>0</v>
@@ -3343,17 +3355,17 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B116" t="s">
-        <v>118</v>
+        <v>21</v>
       </c>
       <c r="C116">
-        <f t="shared" si="2"/>
-        <v>9</v>
+        <f>C115+1</f>
+        <v>97</v>
       </c>
       <c r="D116" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E116" t="b">
         <v>0</v>
@@ -3364,17 +3376,17 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>119</v>
+        <v>29</v>
       </c>
       <c r="C117">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <f>C116+1</f>
+        <v>98</v>
       </c>
       <c r="D117" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E117" t="b">
         <v>0</v>
@@ -3385,17 +3397,17 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>120</v>
+        <v>36</v>
       </c>
       <c r="C118">
-        <f t="shared" si="2"/>
-        <v>11</v>
+        <f>C117+1</f>
+        <v>99</v>
       </c>
       <c r="D118" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E118" t="b">
         <v>0</v>
@@ -3406,17 +3418,17 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B119" t="s">
-        <v>121</v>
+        <v>49</v>
       </c>
       <c r="C119">
-        <f t="shared" si="2"/>
-        <v>12</v>
+        <f>C118+1</f>
+        <v>100</v>
       </c>
       <c r="D119" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E119" t="b">
         <v>0</v>
@@ -3430,14 +3442,14 @@
         <v>70</v>
       </c>
       <c r="B120" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="C120">
-        <f t="shared" si="2"/>
-        <v>13</v>
+        <f>C119+1</f>
+        <v>101</v>
       </c>
       <c r="D120" t="s">
-        <v>172</v>
+        <v>190</v>
       </c>
       <c r="E120" t="b">
         <v>0</v>
@@ -3451,14 +3463,14 @@
         <v>70</v>
       </c>
       <c r="B121" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C121">
-        <f t="shared" si="2"/>
-        <v>14</v>
+        <f>C120+1</f>
+        <v>102</v>
       </c>
       <c r="D121" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E121" t="b">
         <v>0</v>
@@ -3469,17 +3481,17 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B122" t="s">
-        <v>124</v>
+        <v>95</v>
       </c>
       <c r="C122">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f>C121+1</f>
+        <v>103</v>
       </c>
       <c r="D122" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E122" t="b">
         <v>0</v>
@@ -3490,17 +3502,17 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>125</v>
+        <v>26</v>
       </c>
       <c r="C123">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f>C122+1</f>
+        <v>104</v>
       </c>
       <c r="D123" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -3511,17 +3523,17 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>126</v>
+        <v>28</v>
       </c>
       <c r="C124">
-        <f t="shared" si="2"/>
-        <v>17</v>
+        <f>C123+1</f>
+        <v>105</v>
       </c>
       <c r="D124" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
@@ -3532,17 +3544,17 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B125" t="s">
-        <v>127</v>
+        <v>42</v>
       </c>
       <c r="C125">
-        <f t="shared" si="2"/>
-        <v>18</v>
+        <f>C124+1</f>
+        <v>106</v>
       </c>
       <c r="D125" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
@@ -3553,17 +3565,17 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B126" t="s">
-        <v>128</v>
+        <v>68</v>
       </c>
       <c r="C126">
-        <f t="shared" si="2"/>
-        <v>19</v>
+        <f>C125+1</f>
+        <v>107</v>
       </c>
       <c r="D126" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E126" t="b">
         <v>0</v>
@@ -3574,17 +3586,17 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B127" t="s">
-        <v>129</v>
+        <v>87</v>
       </c>
       <c r="C127">
-        <f t="shared" si="2"/>
-        <v>20</v>
+        <f>C126+1</f>
+        <v>108</v>
       </c>
       <c r="D127" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="E127" t="b">
         <v>0</v>
@@ -3598,14 +3610,14 @@
         <v>70</v>
       </c>
       <c r="B128" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C128">
-        <f t="shared" si="2"/>
-        <v>21</v>
+        <f>C127+1</f>
+        <v>109</v>
       </c>
       <c r="D128" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="E128" t="b">
         <v>0</v>
@@ -3616,17 +3628,17 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B129" t="s">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="C129">
-        <f t="shared" si="2"/>
-        <v>22</v>
+        <f>C128+1</f>
+        <v>110</v>
       </c>
       <c r="D129" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E129" t="b">
         <v>0</v>
@@ -3637,17 +3649,17 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B130" t="s">
-        <v>132</v>
+        <v>72</v>
       </c>
       <c r="C130">
-        <f t="shared" si="2"/>
-        <v>23</v>
+        <f>C129+1</f>
+        <v>111</v>
       </c>
       <c r="D130" t="s">
-        <v>165</v>
+        <v>180</v>
       </c>
       <c r="E130" t="b">
         <v>0</v>
@@ -3658,17 +3670,17 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B131" t="s">
-        <v>133</v>
+        <v>79</v>
       </c>
       <c r="C131">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <f>C130+1</f>
+        <v>112</v>
       </c>
       <c r="D131" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="E131" t="b">
         <v>0</v>
@@ -3679,17 +3691,17 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B132" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="C132">
-        <f t="shared" si="2"/>
-        <v>25</v>
+        <f>C131+1</f>
+        <v>113</v>
       </c>
       <c r="D132" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="E132" t="b">
         <v>0</v>
@@ -3703,14 +3715,14 @@
         <v>70</v>
       </c>
       <c r="B133" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="C133">
-        <f t="shared" si="2"/>
-        <v>26</v>
+        <f>C132+1</f>
+        <v>114</v>
       </c>
       <c r="D133" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E133" t="b">
         <v>0</v>
@@ -3724,14 +3736,14 @@
         <v>70</v>
       </c>
       <c r="B134" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C134">
-        <f t="shared" si="2"/>
-        <v>27</v>
+        <f>C133+1</f>
+        <v>115</v>
       </c>
       <c r="D134" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E134" t="b">
         <v>0</v>
@@ -3742,20 +3754,16 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B135" t="s">
-        <v>137</v>
-      </c>
-      <c r="C135">
-        <f t="shared" si="2"/>
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D135" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="E135" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -3763,17 +3771,17 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B136" t="s">
-        <v>138</v>
+        <v>7</v>
       </c>
       <c r="C136">
-        <f t="shared" si="2"/>
-        <v>29</v>
+        <f>C135+1</f>
+        <v>1</v>
       </c>
       <c r="D136" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E136" t="b">
         <v>0</v>
@@ -3784,17 +3792,17 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>139</v>
+        <v>8</v>
       </c>
       <c r="C137">
-        <f t="shared" si="2"/>
-        <v>30</v>
+        <f>C136+1</f>
+        <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>188</v>
+        <v>165</v>
       </c>
       <c r="E137" t="b">
         <v>0</v>
@@ -3805,20 +3813,16 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B138" t="s">
-        <v>140</v>
-      </c>
-      <c r="C138">
-        <f t="shared" si="2"/>
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D138" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E138" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
@@ -3826,17 +3830,17 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B139" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="C139">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f>C138+1</f>
+        <v>1</v>
       </c>
       <c r="D139" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="E139" t="b">
         <v>0</v>
@@ -3847,14 +3851,14 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B140" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="C140">
-        <f t="shared" si="2"/>
-        <v>33</v>
+        <f>C139+1</f>
+        <v>2</v>
       </c>
       <c r="D140" t="s">
         <v>165</v>
@@ -3868,14 +3872,14 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B141" t="s">
-        <v>143</v>
+        <v>73</v>
       </c>
       <c r="C141">
-        <f t="shared" si="2"/>
-        <v>34</v>
+        <f>C140+1</f>
+        <v>3</v>
       </c>
       <c r="D141" t="s">
         <v>165</v>
@@ -3889,17 +3893,17 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B142" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="C142">
-        <f t="shared" si="2"/>
-        <v>35</v>
+        <f>C141+1</f>
+        <v>4</v>
       </c>
       <c r="D142" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="E142" t="b">
         <v>0</v>
@@ -3910,17 +3914,17 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B143" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
       <c r="C143">
-        <f t="shared" si="2"/>
-        <v>36</v>
+        <f>C142+1</f>
+        <v>5</v>
       </c>
       <c r="D143" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="E143" t="b">
         <v>0</v>
@@ -3931,17 +3935,17 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B144" t="s">
-        <v>146</v>
+        <v>110</v>
       </c>
       <c r="C144">
-        <f t="shared" si="2"/>
-        <v>37</v>
+        <f>C143+1</f>
+        <v>6</v>
       </c>
       <c r="D144" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="E144" t="b">
         <v>0</v>
@@ -3955,11 +3959,11 @@
         <v>70</v>
       </c>
       <c r="B145" t="s">
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="C145">
-        <f t="shared" si="2"/>
-        <v>38</v>
+        <f>C144+1</f>
+        <v>7</v>
       </c>
       <c r="D145" t="s">
         <v>165</v>
@@ -3976,11 +3980,11 @@
         <v>70</v>
       </c>
       <c r="B146" t="s">
-        <v>148</v>
+        <v>72</v>
       </c>
       <c r="C146">
-        <f t="shared" si="2"/>
-        <v>39</v>
+        <f>C145+1</f>
+        <v>8</v>
       </c>
       <c r="D146" t="s">
         <v>165</v>
@@ -3997,14 +4001,14 @@
         <v>70</v>
       </c>
       <c r="B147" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C147">
-        <f t="shared" si="2"/>
-        <v>40</v>
+        <f>C146+1</f>
+        <v>9</v>
       </c>
       <c r="D147" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E147" t="b">
         <v>0</v>
@@ -4018,14 +4022,14 @@
         <v>70</v>
       </c>
       <c r="B148" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C148">
-        <f t="shared" si="2"/>
-        <v>41</v>
+        <f>C147+1</f>
+        <v>10</v>
       </c>
       <c r="D148" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E148" t="b">
         <v>0</v>
@@ -4039,14 +4043,14 @@
         <v>70</v>
       </c>
       <c r="B149" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C149">
-        <f t="shared" si="2"/>
-        <v>42</v>
+        <f>C148+1</f>
+        <v>11</v>
       </c>
       <c r="D149" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E149" t="b">
         <v>0</v>
@@ -4060,14 +4064,14 @@
         <v>70</v>
       </c>
       <c r="B150" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C150">
-        <f t="shared" si="2"/>
-        <v>43</v>
+        <f>C149+1</f>
+        <v>12</v>
       </c>
       <c r="D150" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E150" t="b">
         <v>0</v>
@@ -4081,14 +4085,14 @@
         <v>70</v>
       </c>
       <c r="B151" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C151">
-        <f t="shared" si="2"/>
-        <v>44</v>
+        <f>C150+1</f>
+        <v>13</v>
       </c>
       <c r="D151" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E151" t="b">
         <v>0</v>
@@ -4102,14 +4106,14 @@
         <v>70</v>
       </c>
       <c r="B152" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="C152">
-        <f t="shared" si="2"/>
-        <v>45</v>
+        <f>C151+1</f>
+        <v>14</v>
       </c>
       <c r="D152" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E152" t="b">
         <v>0</v>
@@ -4123,14 +4127,14 @@
         <v>70</v>
       </c>
       <c r="B153" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="C153">
-        <f t="shared" si="2"/>
-        <v>46</v>
+        <f>C152+1</f>
+        <v>15</v>
       </c>
       <c r="D153" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="E153" t="b">
         <v>0</v>
@@ -4141,17 +4145,17 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B154" t="s">
-        <v>155</v>
+        <v>31</v>
       </c>
       <c r="C154">
-        <f t="shared" si="2"/>
-        <v>47</v>
+        <f>C153+1</f>
+        <v>16</v>
       </c>
       <c r="D154" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E154" t="b">
         <v>0</v>
@@ -4162,17 +4166,17 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B155" t="s">
-        <v>156</v>
+        <v>37</v>
       </c>
       <c r="C155">
-        <f t="shared" si="2"/>
-        <v>48</v>
+        <f>C154+1</f>
+        <v>17</v>
       </c>
       <c r="D155" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="E155" t="b">
         <v>0</v>
@@ -4183,17 +4187,17 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
+        <v>38</v>
       </c>
       <c r="C156">
-        <f t="shared" si="2"/>
-        <v>49</v>
+        <f>C155+1</f>
+        <v>18</v>
       </c>
       <c r="D156" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E156" t="b">
         <v>0</v>
@@ -4204,17 +4208,17 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B157" t="s">
-        <v>158</v>
+        <v>31</v>
       </c>
       <c r="C157">
-        <f t="shared" si="2"/>
-        <v>50</v>
+        <f>C156+1</f>
+        <v>19</v>
       </c>
       <c r="D157" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E157" t="b">
         <v>0</v>
@@ -4225,17 +4229,17 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B158" t="s">
-        <v>159</v>
+        <v>88</v>
       </c>
       <c r="C158">
-        <f t="shared" si="2"/>
-        <v>51</v>
+        <f>C157+1</f>
+        <v>20</v>
       </c>
       <c r="D158" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="E158" t="b">
         <v>0</v>
@@ -4249,14 +4253,14 @@
         <v>70</v>
       </c>
       <c r="B159" t="s">
-        <v>160</v>
+        <v>114</v>
       </c>
       <c r="C159">
-        <f t="shared" si="2"/>
-        <v>52</v>
+        <f>C158+1</f>
+        <v>21</v>
       </c>
       <c r="D159" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E159" t="b">
         <v>0</v>
@@ -4270,11 +4274,11 @@
         <v>70</v>
       </c>
       <c r="B160" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="C160">
-        <f t="shared" si="2"/>
-        <v>53</v>
+        <f>C159+1</f>
+        <v>22</v>
       </c>
       <c r="D160" t="s">
         <v>176</v>
@@ -4291,14 +4295,14 @@
         <v>70</v>
       </c>
       <c r="B161" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C161">
         <f>C160+1</f>
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D161" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E161" t="b">
         <v>0</v>
@@ -4312,14 +4316,14 @@
         <v>70</v>
       </c>
       <c r="B162" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C162">
-        <f t="shared" si="2"/>
-        <v>55</v>
+        <f>C161+1</f>
+        <v>24</v>
       </c>
       <c r="D162" t="s">
-        <v>193</v>
+        <v>176</v>
       </c>
       <c r="E162" t="b">
         <v>0</v>
@@ -4333,20 +4337,191 @@
         <v>70</v>
       </c>
       <c r="B163" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C163">
-        <f t="shared" si="2"/>
-        <v>56</v>
+        <f>C162+1</f>
+        <v>25</v>
       </c>
       <c r="D163" t="s">
+        <v>176</v>
+      </c>
+      <c r="E163" t="b">
+        <v>0</v>
+      </c>
+      <c r="F163" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F163">
+    <sortCondition ref="D1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>165</v>
       </c>
-      <c r="E163" t="b">
-        <v>0</v>
-      </c>
-      <c r="F163" t="b">
-        <v>0</v>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ChapterIcon tab in data collection, this time without my screwing up the chapter list;
</commit_message>
<xml_diff>
--- a/Data/Chapters.xlsx
+++ b/Data/Chapters.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
   </bookViews>
   <sheets>
     <sheet name="Chapter" sheetId="1" r:id="rId1"/>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F163"/>
   <sheetViews>
-    <sheetView topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D163"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,20 +965,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C2" t="e">
-        <f>C1+1</f>
-        <v>#VALUE!</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" t="b">
         <v>0</v>
@@ -986,17 +982,17 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C3" t="e">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <f>C2+1</f>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -1010,14 +1006,14 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" t="e">
-        <f>C3+1</f>
-        <v>#VALUE!</v>
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C55" si="0">C3+1</f>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -1031,14 +1027,14 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="e">
-        <f>C4+1</f>
-        <v>#VALUE!</v>
+        <v>11</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -1049,17 +1045,17 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
-      </c>
-      <c r="C6" t="e">
-        <f>C5+1</f>
-        <v>#VALUE!</v>
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -1070,17 +1066,17 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" t="e">
-        <f>C6+1</f>
-        <v>#VALUE!</v>
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -1091,17 +1087,17 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8" t="e">
-        <f>C7+1</f>
-        <v>#VALUE!</v>
+        <v>14</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
@@ -1112,17 +1108,17 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
-      </c>
-      <c r="C9" t="e">
-        <f>C8+1</f>
-        <v>#VALUE!</v>
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -1136,14 +1132,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" t="e">
-        <f>C9+1</f>
-        <v>#VALUE!</v>
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
@@ -1157,14 +1153,14 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" t="e">
-        <f>C10+1</f>
-        <v>#VALUE!</v>
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -1175,17 +1171,17 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" t="e">
-        <f>C11+1</f>
-        <v>#VALUE!</v>
+        <v>18</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
@@ -1196,17 +1192,17 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" t="e">
-        <f>C12+1</f>
-        <v>#VALUE!</v>
+        <v>19</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -1217,17 +1213,17 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" t="e">
-        <f>C13+1</f>
-        <v>#VALUE!</v>
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
@@ -1238,17 +1234,17 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" t="e">
-        <f>C14+1</f>
-        <v>#VALUE!</v>
+        <v>21</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
@@ -1262,14 +1258,14 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="e">
-        <f>C15+1</f>
-        <v>#VALUE!</v>
+        <v>22</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
@@ -1283,11 +1279,11 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" t="e">
-        <f>C16+1</f>
-        <v>#VALUE!</v>
+        <v>23</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="D17" t="s">
         <v>173</v>
@@ -1301,17 +1297,17 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="e">
-        <f>C17+1</f>
-        <v>#VALUE!</v>
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
@@ -1322,16 +1318,20 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B19" t="s">
-        <v>111</v>
+        <v>25</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="b">
         <v>0</v>
@@ -1339,17 +1339,17 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
+        <v>26</v>
       </c>
       <c r="C20">
-        <f>C19+1</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
@@ -1360,17 +1360,17 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C21">
-        <f>C20+1</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
       <c r="D21" t="s">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
@@ -1381,17 +1381,17 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>28</v>
       </c>
       <c r="C22">
-        <f>C21+1</f>
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
@@ -1402,17 +1402,17 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B23" t="s">
-        <v>101</v>
+        <v>29</v>
       </c>
       <c r="C23">
-        <f>C22+1</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
@@ -1423,17 +1423,17 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B24" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="C24">
-        <f>C23+1</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
@@ -1447,14 +1447,14 @@
         <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C25">
-        <f>C24+1</f>
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="E25" t="b">
         <v>0</v>
@@ -1468,14 +1468,14 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="C26">
-        <f>C25+1</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E26" t="b">
         <v>0</v>
@@ -1489,14 +1489,14 @@
         <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C27">
-        <f>C26+1</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>25</v>
       </c>
       <c r="D27" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
@@ -1510,14 +1510,14 @@
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C28">
-        <f>C27+1</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
@@ -1531,14 +1531,14 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="C29">
-        <f>C28+1</f>
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
@@ -1549,17 +1549,17 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>36</v>
       </c>
       <c r="C30">
-        <f>C29+1</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
@@ -1570,17 +1570,17 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>37</v>
       </c>
       <c r="C31">
-        <f>C30+1</f>
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
@@ -1591,17 +1591,17 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>38</v>
       </c>
       <c r="C32">
-        <f>C31+1</f>
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -1612,17 +1612,17 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>139</v>
+        <v>39</v>
       </c>
       <c r="C33">
-        <f>C32+1</f>
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>31</v>
       </c>
       <c r="D33" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -1633,17 +1633,17 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>40</v>
       </c>
       <c r="C34">
-        <f>C33+1</f>
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -1654,17 +1654,17 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
       <c r="C35">
-        <f>C34+1</f>
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>33</v>
       </c>
       <c r="D35" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -1675,17 +1675,17 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>162</v>
+        <v>42</v>
       </c>
       <c r="C36">
-        <f>C35+1</f>
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
@@ -1696,17 +1696,17 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>43</v>
       </c>
       <c r="C37">
-        <f>C36+1</f>
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
@@ -1717,17 +1717,17 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>123</v>
+        <v>44</v>
       </c>
       <c r="C38">
-        <f>C37+1</f>
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
       <c r="D38" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
@@ -1738,17 +1738,17 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="C39">
-        <f>C38+1</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>37</v>
       </c>
       <c r="D39" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
@@ -1759,17 +1759,17 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>135</v>
+        <v>46</v>
       </c>
       <c r="C40">
-        <f>C39+1</f>
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
@@ -1780,17 +1780,17 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
       <c r="C41">
-        <f>C40+1</f>
-        <v>22</v>
+        <f t="shared" si="0"/>
+        <v>39</v>
       </c>
       <c r="D41" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -1804,14 +1804,14 @@
         <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C42">
-        <f>C41+1</f>
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>40</v>
       </c>
       <c r="D42" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -1825,14 +1825,14 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="C43">
-        <f>C42+1</f>
-        <v>24</v>
+        <f t="shared" si="0"/>
+        <v>41</v>
       </c>
       <c r="D43" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -1846,14 +1846,14 @@
         <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>22</v>
+        <v>50</v>
       </c>
       <c r="C44">
-        <f>C43+1</f>
-        <v>25</v>
+        <f t="shared" si="0"/>
+        <v>42</v>
       </c>
       <c r="D44" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
@@ -1867,11 +1867,11 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="C45">
-        <f>C44+1</f>
-        <v>26</v>
+        <f t="shared" si="0"/>
+        <v>43</v>
       </c>
       <c r="D45" t="s">
         <v>167</v>
@@ -1888,14 +1888,14 @@
         <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C46">
-        <f>C45+1</f>
-        <v>27</v>
+        <f t="shared" si="0"/>
+        <v>44</v>
       </c>
       <c r="D46" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -1909,11 +1909,11 @@
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C47">
-        <f>C46+1</f>
-        <v>28</v>
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
       <c r="D47" t="s">
         <v>167</v>
@@ -1930,14 +1930,14 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C48">
-        <f>C47+1</f>
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E48" t="b">
         <v>0</v>
@@ -1948,17 +1948,17 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C49">
-        <f>C48+1</f>
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>47</v>
       </c>
       <c r="D49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E49" t="b">
         <v>0</v>
@@ -1969,17 +1969,17 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="C50">
-        <f>C49+1</f>
-        <v>31</v>
+        <f t="shared" si="0"/>
+        <v>48</v>
       </c>
       <c r="D50" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
@@ -1990,17 +1990,17 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="C51">
-        <f>C50+1</f>
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
@@ -2011,17 +2011,17 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="C52">
-        <f>C51+1</f>
-        <v>33</v>
+        <f t="shared" si="0"/>
+        <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E52" t="b">
         <v>0</v>
@@ -2032,17 +2032,17 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="C53">
-        <f>C52+1</f>
-        <v>34</v>
+        <f t="shared" si="0"/>
+        <v>51</v>
       </c>
       <c r="D53" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E53" t="b">
         <v>0</v>
@@ -2053,17 +2053,17 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>60</v>
       </c>
       <c r="C54">
-        <f>C53+1</f>
-        <v>35</v>
+        <f t="shared" si="0"/>
+        <v>52</v>
       </c>
       <c r="D54" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -2074,17 +2074,17 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>8</v>
       </c>
       <c r="C55">
-        <f>C54+1</f>
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E55" t="b">
         <v>0</v>
@@ -2095,20 +2095,16 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C56">
-        <f>C55+1</f>
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E56" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F56" t="b">
         <v>0</v>
@@ -2116,17 +2112,17 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C57">
         <f>C56+1</f>
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E57" t="b">
         <v>0</v>
@@ -2137,14 +2133,14 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="C58">
-        <f>C57+1</f>
-        <v>39</v>
+        <f t="shared" ref="C58:C106" si="1">C57+1</f>
+        <v>2</v>
       </c>
       <c r="D58" t="s">
         <v>172</v>
@@ -2161,14 +2157,14 @@
         <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C59">
-        <f>C58+1</f>
-        <v>40</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="D59" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -2182,14 +2178,14 @@
         <v>61</v>
       </c>
       <c r="B60" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C60">
-        <f>C59+1</f>
-        <v>41</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="D60" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E60" t="b">
         <v>0</v>
@@ -2203,14 +2199,14 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C61">
-        <f>C60+1</f>
-        <v>42</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -2224,14 +2220,14 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C62">
-        <f>C61+1</f>
-        <v>43</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="D62" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="E62" t="b">
         <v>0</v>
@@ -2245,14 +2241,14 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C63">
-        <f>C62+1</f>
-        <v>44</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="D63" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E63" t="b">
         <v>0</v>
@@ -2266,14 +2262,14 @@
         <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C64">
-        <f>C63+1</f>
-        <v>45</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="D64" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -2287,11 +2283,11 @@
         <v>61</v>
       </c>
       <c r="B65" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="C65">
-        <f>C64+1</f>
-        <v>46</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
       </c>
       <c r="D65" t="s">
         <v>172</v>
@@ -2308,14 +2304,14 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
       <c r="C66">
-        <f>C65+1</f>
-        <v>47</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="D66" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="E66" t="b">
         <v>0</v>
@@ -2326,17 +2322,17 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B67" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="C67">
-        <f>C66+1</f>
-        <v>48</v>
+        <f t="shared" si="1"/>
+        <v>11</v>
       </c>
       <c r="D67" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="E67" t="b">
         <v>0</v>
@@ -2347,14 +2343,14 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
+        <v>74</v>
       </c>
       <c r="C68">
-        <f>C67+1</f>
-        <v>49</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="D68" t="s">
         <v>172</v>
@@ -2368,17 +2364,17 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>75</v>
       </c>
       <c r="C69">
-        <f>C68+1</f>
-        <v>50</v>
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
       <c r="D69" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -2389,17 +2385,17 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>122</v>
+        <v>31</v>
       </c>
       <c r="C70">
-        <f>C69+1</f>
-        <v>51</v>
+        <f t="shared" si="1"/>
+        <v>14</v>
       </c>
       <c r="D70" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E70" t="b">
         <v>0</v>
@@ -2410,17 +2406,17 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B71" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="C71">
-        <f>C70+1</f>
-        <v>52</v>
+        <f t="shared" si="1"/>
+        <v>15</v>
       </c>
       <c r="D71" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E71" t="b">
         <v>0</v>
@@ -2431,17 +2427,17 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>131</v>
+        <v>77</v>
       </c>
       <c r="C72">
-        <f>C71+1</f>
-        <v>53</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="D72" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E72" t="b">
         <v>0</v>
@@ -2452,17 +2448,17 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>21</v>
       </c>
       <c r="C73">
-        <f>C72+1</f>
-        <v>54</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="D73" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="E73" t="b">
         <v>0</v>
@@ -2473,14 +2469,14 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="C74">
-        <f>C73+1</f>
-        <v>55</v>
+        <f t="shared" si="1"/>
+        <v>18</v>
       </c>
       <c r="D74" t="s">
         <v>172</v>
@@ -2494,17 +2490,17 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
-        <v>12</v>
+        <v>79</v>
       </c>
       <c r="C75">
-        <f>C74+1</f>
-        <v>56</v>
+        <f t="shared" si="1"/>
+        <v>19</v>
       </c>
       <c r="D75" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="E75" t="b">
         <v>0</v>
@@ -2515,17 +2511,17 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B76" t="s">
-        <v>32</v>
+        <v>80</v>
       </c>
       <c r="C76">
-        <f>C75+1</f>
-        <v>57</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="D76" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E76" t="b">
         <v>0</v>
@@ -2536,14 +2532,14 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B77" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
       <c r="C77">
-        <f>C76+1</f>
-        <v>58</v>
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
       <c r="D77" t="s">
         <v>168</v>
@@ -2560,14 +2556,14 @@
         <v>61</v>
       </c>
       <c r="B78" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C78">
-        <f>C77+1</f>
-        <v>59</v>
+        <f t="shared" si="1"/>
+        <v>22</v>
       </c>
       <c r="D78" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E78" t="b">
         <v>0</v>
@@ -2581,14 +2577,14 @@
         <v>61</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C79">
-        <f>C78+1</f>
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E79" t="b">
         <v>0</v>
@@ -2602,14 +2598,14 @@
         <v>61</v>
       </c>
       <c r="B80" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C80">
-        <f>C79+1</f>
-        <v>61</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="D80" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E80" t="b">
         <v>0</v>
@@ -2620,17 +2616,17 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B81" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="C81">
-        <f>C80+1</f>
-        <v>62</v>
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E81" t="b">
         <v>0</v>
@@ -2641,14 +2637,14 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B82" t="s">
-        <v>160</v>
+        <v>86</v>
       </c>
       <c r="C82">
-        <f>C81+1</f>
-        <v>63</v>
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
       <c r="D82" t="s">
         <v>168</v>
@@ -2662,17 +2658,17 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B83" t="s">
-        <v>14</v>
+        <v>87</v>
       </c>
       <c r="C83">
-        <f>C82+1</f>
-        <v>64</v>
+        <f t="shared" si="1"/>
+        <v>27</v>
       </c>
       <c r="D83" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="E83" t="b">
         <v>0</v>
@@ -2683,17 +2679,17 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B84" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="C84">
-        <f>C83+1</f>
-        <v>65</v>
+        <f t="shared" si="1"/>
+        <v>28</v>
       </c>
       <c r="D84" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="E84" t="b">
         <v>0</v>
@@ -2704,17 +2700,17 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="C85">
-        <f>C84+1</f>
-        <v>66</v>
+        <f t="shared" si="1"/>
+        <v>29</v>
       </c>
       <c r="D85" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="E85" t="b">
         <v>0</v>
@@ -2725,17 +2721,17 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B86" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="C86">
-        <f>C85+1</f>
-        <v>67</v>
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
       <c r="D86" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="E86" t="b">
         <v>0</v>
@@ -2749,14 +2745,14 @@
         <v>61</v>
       </c>
       <c r="B87" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="C87">
-        <f>C86+1</f>
-        <v>68</v>
+        <f t="shared" si="1"/>
+        <v>31</v>
       </c>
       <c r="D87" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="E87" t="b">
         <v>0</v>
@@ -2770,14 +2766,14 @@
         <v>61</v>
       </c>
       <c r="B88" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C88">
-        <f>C87+1</f>
-        <v>69</v>
+        <f t="shared" si="1"/>
+        <v>32</v>
       </c>
       <c r="D88" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E88" t="b">
         <v>0</v>
@@ -2788,17 +2784,17 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B89" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="C89">
-        <f>C88+1</f>
-        <v>70</v>
+        <f t="shared" si="1"/>
+        <v>33</v>
       </c>
       <c r="D89" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="E89" t="b">
         <v>0</v>
@@ -2809,17 +2805,17 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B90" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="C90">
-        <f>C89+1</f>
-        <v>71</v>
+        <f t="shared" si="1"/>
+        <v>34</v>
       </c>
       <c r="D90" t="s">
-        <v>189</v>
+        <v>165</v>
       </c>
       <c r="E90" t="b">
         <v>0</v>
@@ -2830,17 +2826,17 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B91" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="C91">
-        <f>C90+1</f>
-        <v>72</v>
+        <f t="shared" si="1"/>
+        <v>35</v>
       </c>
       <c r="D91" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="E91" t="b">
         <v>0</v>
@@ -2851,17 +2847,17 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B92" t="s">
-        <v>145</v>
+        <v>96</v>
       </c>
       <c r="C92">
-        <f>C91+1</f>
-        <v>73</v>
+        <f t="shared" si="1"/>
+        <v>36</v>
       </c>
       <c r="D92" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E92" t="b">
         <v>0</v>
@@ -2872,17 +2868,17 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B93" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="C93">
         <f>C92+1</f>
-        <v>74</v>
+        <v>37</v>
       </c>
       <c r="D93" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="E93" t="b">
         <v>0</v>
@@ -2893,17 +2889,17 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="C94">
-        <f>C93+1</f>
-        <v>75</v>
+        <f t="shared" si="1"/>
+        <v>38</v>
       </c>
       <c r="D94" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
@@ -2914,17 +2910,17 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B95" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="C95">
-        <f>C94+1</f>
-        <v>76</v>
+        <f t="shared" si="1"/>
+        <v>39</v>
       </c>
       <c r="D95" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -2935,17 +2931,17 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B96" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="C96">
-        <f>C95+1</f>
-        <v>77</v>
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="D96" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="E96" t="b">
         <v>0</v>
@@ -2956,17 +2952,17 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
       <c r="C97">
-        <f>C96+1</f>
-        <v>78</v>
+        <f t="shared" si="1"/>
+        <v>41</v>
       </c>
       <c r="D97" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E97" t="b">
         <v>0</v>
@@ -2977,17 +2973,17 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B98" t="s">
-        <v>58</v>
+        <v>102</v>
       </c>
       <c r="C98">
-        <f>C97+1</f>
-        <v>79</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="D98" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="E98" t="b">
         <v>0</v>
@@ -2998,17 +2994,17 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B99" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="C99">
-        <f>C98+1</f>
-        <v>80</v>
+        <f t="shared" si="1"/>
+        <v>43</v>
       </c>
       <c r="D99" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="E99" t="b">
         <v>0</v>
@@ -3022,14 +3018,14 @@
         <v>61</v>
       </c>
       <c r="B100" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="C100">
-        <f>C99+1</f>
-        <v>81</v>
+        <f t="shared" si="1"/>
+        <v>44</v>
       </c>
       <c r="D100" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="E100" t="b">
         <v>0</v>
@@ -3043,14 +3039,14 @@
         <v>61</v>
       </c>
       <c r="B101" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C101">
-        <f>C100+1</f>
-        <v>82</v>
+        <f t="shared" si="1"/>
+        <v>45</v>
       </c>
       <c r="D101" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="E101" t="b">
         <v>0</v>
@@ -3064,14 +3060,14 @@
         <v>61</v>
       </c>
       <c r="B102" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="C102">
-        <f>C101+1</f>
-        <v>83</v>
+        <f t="shared" si="1"/>
+        <v>46</v>
       </c>
       <c r="D102" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E102" t="b">
         <v>0</v>
@@ -3082,17 +3078,17 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B103" t="s">
-        <v>156</v>
+        <v>107</v>
       </c>
       <c r="C103">
-        <f>C102+1</f>
-        <v>84</v>
+        <f t="shared" si="1"/>
+        <v>47</v>
       </c>
       <c r="D103" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="E103" t="b">
         <v>0</v>
@@ -3106,14 +3102,14 @@
         <v>61</v>
       </c>
       <c r="B104" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
       <c r="C104">
         <f>C103+1</f>
-        <v>85</v>
+        <v>48</v>
       </c>
       <c r="D104" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E104" t="b">
         <v>0</v>
@@ -3127,14 +3123,14 @@
         <v>61</v>
       </c>
       <c r="B105" t="s">
-        <v>21</v>
+        <v>109</v>
       </c>
       <c r="C105">
-        <f>C104+1</f>
-        <v>86</v>
+        <f t="shared" si="1"/>
+        <v>49</v>
       </c>
       <c r="D105" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="E105" t="b">
         <v>0</v>
@@ -3148,14 +3144,14 @@
         <v>61</v>
       </c>
       <c r="B106" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="C106">
-        <f>C105+1</f>
-        <v>87</v>
+        <f t="shared" si="1"/>
+        <v>50</v>
       </c>
       <c r="D106" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="E106" t="b">
         <v>0</v>
@@ -3166,20 +3162,16 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B107" t="s">
-        <v>10</v>
-      </c>
-      <c r="C107">
-        <f>C106+1</f>
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="D107" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="E107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" t="b">
         <v>0</v>
@@ -3187,14 +3179,14 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B108" t="s">
-        <v>27</v>
+        <v>112</v>
       </c>
       <c r="C108">
         <f>C107+1</f>
-        <v>89</v>
+        <v>1</v>
       </c>
       <c r="D108" t="s">
         <v>166</v>
@@ -3208,17 +3200,17 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B109" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="C109">
-        <f>C108+1</f>
-        <v>90</v>
+        <f t="shared" ref="C109:C163" si="2">C108+1</f>
+        <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -3229,17 +3221,17 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B110" t="s">
-        <v>55</v>
+        <v>113</v>
       </c>
       <c r="C110">
-        <f>C109+1</f>
-        <v>91</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="D110" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E110" t="b">
         <v>0</v>
@@ -3253,14 +3245,14 @@
         <v>70</v>
       </c>
       <c r="B111" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C111">
-        <f>C110+1</f>
-        <v>92</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="D111" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
@@ -3271,17 +3263,17 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B112" t="s">
-        <v>89</v>
+        <v>115</v>
       </c>
       <c r="C112">
-        <f>C111+1</f>
-        <v>93</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
       <c r="D112" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
@@ -3292,17 +3284,17 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B113" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C113">
-        <f>C112+1</f>
-        <v>94</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
       <c r="D113" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -3313,17 +3305,17 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B114" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C114">
-        <f>C113+1</f>
-        <v>95</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
       </c>
       <c r="D114" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E114" t="b">
         <v>0</v>
@@ -3334,17 +3326,17 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B115" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="C115">
-        <f>C114+1</f>
-        <v>96</v>
+        <f t="shared" si="2"/>
+        <v>8</v>
       </c>
       <c r="D115" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="E115" t="b">
         <v>0</v>
@@ -3355,17 +3347,17 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B116" t="s">
-        <v>21</v>
+        <v>118</v>
       </c>
       <c r="C116">
-        <f>C115+1</f>
-        <v>97</v>
+        <f t="shared" si="2"/>
+        <v>9</v>
       </c>
       <c r="D116" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="E116" t="b">
         <v>0</v>
@@ -3376,17 +3368,17 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B117" t="s">
-        <v>29</v>
+        <v>119</v>
       </c>
       <c r="C117">
-        <f>C116+1</f>
-        <v>98</v>
+        <f t="shared" si="2"/>
+        <v>10</v>
       </c>
       <c r="D117" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E117" t="b">
         <v>0</v>
@@ -3397,17 +3389,17 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B118" t="s">
-        <v>36</v>
+        <v>120</v>
       </c>
       <c r="C118">
-        <f>C117+1</f>
-        <v>99</v>
+        <f t="shared" si="2"/>
+        <v>11</v>
       </c>
       <c r="D118" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E118" t="b">
         <v>0</v>
@@ -3418,17 +3410,17 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B119" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="C119">
-        <f>C118+1</f>
-        <v>100</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="D119" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="E119" t="b">
         <v>0</v>
@@ -3442,14 +3434,14 @@
         <v>70</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C120">
-        <f>C119+1</f>
-        <v>101</v>
+        <f t="shared" si="2"/>
+        <v>13</v>
       </c>
       <c r="D120" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="E120" t="b">
         <v>0</v>
@@ -3463,14 +3455,14 @@
         <v>70</v>
       </c>
       <c r="B121" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C121">
-        <f>C120+1</f>
-        <v>102</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="D121" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E121" t="b">
         <v>0</v>
@@ -3481,17 +3473,17 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B122" t="s">
-        <v>95</v>
+        <v>124</v>
       </c>
       <c r="C122">
-        <f>C121+1</f>
-        <v>103</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="D122" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E122" t="b">
         <v>0</v>
@@ -3502,17 +3494,17 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B123" t="s">
-        <v>26</v>
+        <v>125</v>
       </c>
       <c r="C123">
-        <f>C122+1</f>
-        <v>104</v>
+        <f t="shared" si="2"/>
+        <v>16</v>
       </c>
       <c r="D123" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -3523,17 +3515,17 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B124" t="s">
-        <v>28</v>
+        <v>126</v>
       </c>
       <c r="C124">
-        <f>C123+1</f>
-        <v>105</v>
+        <f t="shared" si="2"/>
+        <v>17</v>
       </c>
       <c r="D124" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
@@ -3544,17 +3536,17 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B125" t="s">
-        <v>42</v>
+        <v>127</v>
       </c>
       <c r="C125">
-        <f>C124+1</f>
-        <v>106</v>
+        <f t="shared" si="2"/>
+        <v>18</v>
       </c>
       <c r="D125" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
@@ -3565,17 +3557,17 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B126" t="s">
-        <v>68</v>
+        <v>128</v>
       </c>
       <c r="C126">
-        <f>C125+1</f>
-        <v>107</v>
+        <f t="shared" si="2"/>
+        <v>19</v>
       </c>
       <c r="D126" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="E126" t="b">
         <v>0</v>
@@ -3586,17 +3578,17 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B127" t="s">
-        <v>87</v>
+        <v>129</v>
       </c>
       <c r="C127">
-        <f>C126+1</f>
-        <v>108</v>
+        <f t="shared" si="2"/>
+        <v>20</v>
       </c>
       <c r="D127" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E127" t="b">
         <v>0</v>
@@ -3610,14 +3602,14 @@
         <v>70</v>
       </c>
       <c r="B128" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C128">
-        <f>C127+1</f>
-        <v>109</v>
+        <f t="shared" si="2"/>
+        <v>21</v>
       </c>
       <c r="D128" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="E128" t="b">
         <v>0</v>
@@ -3628,17 +3620,17 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B129" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="C129">
-        <f>C128+1</f>
-        <v>110</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="D129" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="E129" t="b">
         <v>0</v>
@@ -3649,17 +3641,17 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B130" t="s">
-        <v>72</v>
+        <v>132</v>
       </c>
       <c r="C130">
-        <f>C129+1</f>
-        <v>111</v>
+        <f t="shared" si="2"/>
+        <v>23</v>
       </c>
       <c r="D130" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="E130" t="b">
         <v>0</v>
@@ -3670,17 +3662,17 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B131" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="C131">
-        <f>C130+1</f>
-        <v>112</v>
+        <f t="shared" si="2"/>
+        <v>24</v>
       </c>
       <c r="D131" t="s">
-        <v>180</v>
+        <v>188</v>
       </c>
       <c r="E131" t="b">
         <v>0</v>
@@ -3691,17 +3683,17 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B132" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="C132">
-        <f>C131+1</f>
-        <v>113</v>
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
       <c r="D132" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="E132" t="b">
         <v>0</v>
@@ -3715,14 +3707,14 @@
         <v>70</v>
       </c>
       <c r="B133" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C133">
-        <f>C132+1</f>
-        <v>114</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="D133" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E133" t="b">
         <v>0</v>
@@ -3736,14 +3728,14 @@
         <v>70</v>
       </c>
       <c r="B134" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C134">
-        <f>C133+1</f>
-        <v>115</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
       <c r="D134" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E134" t="b">
         <v>0</v>
@@ -3754,16 +3746,20 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>137</v>
+      </c>
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>28</v>
       </c>
       <c r="D135" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="E135" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F135" t="b">
         <v>0</v>
@@ -3771,17 +3767,17 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>138</v>
       </c>
       <c r="C136">
-        <f>C135+1</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>29</v>
       </c>
       <c r="D136" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E136" t="b">
         <v>0</v>
@@ -3792,17 +3788,17 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B137" t="s">
-        <v>8</v>
+        <v>139</v>
       </c>
       <c r="C137">
-        <f>C136+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="D137" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="E137" t="b">
         <v>0</v>
@@ -3813,16 +3809,20 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B138" t="s">
-        <v>62</v>
+        <v>140</v>
+      </c>
+      <c r="C138">
+        <f t="shared" si="2"/>
+        <v>31</v>
       </c>
       <c r="D138" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="E138" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F138" t="b">
         <v>0</v>
@@ -3830,17 +3830,17 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B139" t="s">
-        <v>63</v>
+        <v>141</v>
       </c>
       <c r="C139">
-        <f>C138+1</f>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>32</v>
       </c>
       <c r="D139" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="E139" t="b">
         <v>0</v>
@@ -3851,14 +3851,14 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B140" t="s">
-        <v>69</v>
+        <v>142</v>
       </c>
       <c r="C140">
-        <f>C139+1</f>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>33</v>
       </c>
       <c r="D140" t="s">
         <v>165</v>
@@ -3872,14 +3872,14 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B141" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="C141">
-        <f>C140+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
       <c r="D141" t="s">
         <v>165</v>
@@ -3893,17 +3893,17 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B142" t="s">
-        <v>94</v>
+        <v>144</v>
       </c>
       <c r="C142">
-        <f>C141+1</f>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>35</v>
       </c>
       <c r="D142" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
       <c r="E142" t="b">
         <v>0</v>
@@ -3914,17 +3914,17 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B143" t="s">
-        <v>109</v>
+        <v>145</v>
       </c>
       <c r="C143">
-        <f>C142+1</f>
-        <v>5</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="D143" t="s">
-        <v>165</v>
+        <v>192</v>
       </c>
       <c r="E143" t="b">
         <v>0</v>
@@ -3935,17 +3935,17 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B144" t="s">
-        <v>110</v>
+        <v>146</v>
       </c>
       <c r="C144">
-        <f>C143+1</f>
-        <v>6</v>
+        <f t="shared" si="2"/>
+        <v>37</v>
       </c>
       <c r="D144" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="E144" t="b">
         <v>0</v>
@@ -3959,11 +3959,11 @@
         <v>70</v>
       </c>
       <c r="B145" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
       <c r="C145">
-        <f>C144+1</f>
-        <v>7</v>
+        <f t="shared" si="2"/>
+        <v>38</v>
       </c>
       <c r="D145" t="s">
         <v>165</v>
@@ -3980,11 +3980,11 @@
         <v>70</v>
       </c>
       <c r="B146" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="C146">
-        <f>C145+1</f>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>39</v>
       </c>
       <c r="D146" t="s">
         <v>165</v>
@@ -4001,14 +4001,14 @@
         <v>70</v>
       </c>
       <c r="B147" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="C147">
-        <f>C146+1</f>
-        <v>9</v>
+        <f t="shared" si="2"/>
+        <v>40</v>
       </c>
       <c r="D147" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="E147" t="b">
         <v>0</v>
@@ -4022,14 +4022,14 @@
         <v>70</v>
       </c>
       <c r="B148" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="C148">
-        <f>C147+1</f>
-        <v>10</v>
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
       <c r="D148" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E148" t="b">
         <v>0</v>
@@ -4043,14 +4043,14 @@
         <v>70</v>
       </c>
       <c r="B149" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C149">
-        <f>C148+1</f>
-        <v>11</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="D149" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E149" t="b">
         <v>0</v>
@@ -4064,14 +4064,14 @@
         <v>70</v>
       </c>
       <c r="B150" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C150">
-        <f>C149+1</f>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>43</v>
       </c>
       <c r="D150" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="E150" t="b">
         <v>0</v>
@@ -4085,14 +4085,14 @@
         <v>70</v>
       </c>
       <c r="B151" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C151">
-        <f>C150+1</f>
-        <v>13</v>
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="D151" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="E151" t="b">
         <v>0</v>
@@ -4106,14 +4106,14 @@
         <v>70</v>
       </c>
       <c r="B152" t="s">
-        <v>158</v>
+        <v>43</v>
       </c>
       <c r="C152">
-        <f>C151+1</f>
-        <v>14</v>
+        <f t="shared" si="2"/>
+        <v>45</v>
       </c>
       <c r="D152" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="E152" t="b">
         <v>0</v>
@@ -4127,14 +4127,14 @@
         <v>70</v>
       </c>
       <c r="B153" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C153">
-        <f>C152+1</f>
-        <v>15</v>
+        <f t="shared" si="2"/>
+        <v>46</v>
       </c>
       <c r="D153" t="s">
-        <v>165</v>
+        <v>177</v>
       </c>
       <c r="E153" t="b">
         <v>0</v>
@@ -4145,17 +4145,17 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B154" t="s">
-        <v>31</v>
+        <v>155</v>
       </c>
       <c r="C154">
-        <f>C153+1</f>
-        <v>16</v>
+        <f t="shared" si="2"/>
+        <v>47</v>
       </c>
       <c r="D154" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E154" t="b">
         <v>0</v>
@@ -4166,17 +4166,17 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B155" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
       <c r="C155">
-        <f>C154+1</f>
-        <v>17</v>
+        <f t="shared" si="2"/>
+        <v>48</v>
       </c>
       <c r="D155" t="s">
-        <v>176</v>
+        <v>184</v>
       </c>
       <c r="E155" t="b">
         <v>0</v>
@@ -4187,17 +4187,17 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="B156" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
       <c r="C156">
-        <f>C155+1</f>
-        <v>18</v>
+        <f t="shared" si="2"/>
+        <v>49</v>
       </c>
       <c r="D156" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E156" t="b">
         <v>0</v>
@@ -4208,17 +4208,17 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B157" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="C157">
-        <f>C156+1</f>
-        <v>19</v>
+        <f t="shared" si="2"/>
+        <v>50</v>
       </c>
       <c r="D157" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E157" t="b">
         <v>0</v>
@@ -4229,17 +4229,17 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B158" t="s">
-        <v>88</v>
+        <v>159</v>
       </c>
       <c r="C158">
-        <f>C157+1</f>
-        <v>20</v>
+        <f t="shared" si="2"/>
+        <v>51</v>
       </c>
       <c r="D158" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="E158" t="b">
         <v>0</v>
@@ -4253,14 +4253,14 @@
         <v>70</v>
       </c>
       <c r="B159" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="C159">
-        <f>C158+1</f>
-        <v>21</v>
+        <f t="shared" si="2"/>
+        <v>52</v>
       </c>
       <c r="D159" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="E159" t="b">
         <v>0</v>
@@ -4274,11 +4274,11 @@
         <v>70</v>
       </c>
       <c r="B160" t="s">
-        <v>117</v>
+        <v>161</v>
       </c>
       <c r="C160">
-        <f>C159+1</f>
-        <v>22</v>
+        <f t="shared" si="2"/>
+        <v>53</v>
       </c>
       <c r="D160" t="s">
         <v>176</v>
@@ -4295,14 +4295,14 @@
         <v>70</v>
       </c>
       <c r="B161" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="C161">
         <f>C160+1</f>
-        <v>23</v>
+        <v>54</v>
       </c>
       <c r="D161" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="E161" t="b">
         <v>0</v>
@@ -4316,14 +4316,14 @@
         <v>70</v>
       </c>
       <c r="B162" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="C162">
-        <f>C161+1</f>
-        <v>24</v>
+        <f t="shared" si="2"/>
+        <v>55</v>
       </c>
       <c r="D162" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="E162" t="b">
         <v>0</v>
@@ -4337,14 +4337,14 @@
         <v>70</v>
       </c>
       <c r="B163" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C163">
-        <f>C162+1</f>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>56</v>
       </c>
       <c r="D163" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="E163" t="b">
         <v>0</v>
@@ -4354,9 +4354,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F163">
-    <sortCondition ref="D1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4365,8 +4362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>